<commit_message>
[MS-OXWSMSG] Update capture code according to watchman report
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source Depot\Repos\Interop-TestSuites-1\ExchangeWebServices\Docs\MS-OXWSMSG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Interop_TestSuites\ExchangeWebServices\Docs\MS-OXWSMSG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="590">
   <si>
     <t>Req ID</t>
   </si>
@@ -1778,9 +1778,6 @@
     </r>
   </si>
   <si>
-    <t>[In Transport] This protocol uses SOAP 1.1.</t>
-  </si>
-  <si>
     <t>The endpoint URL that is returned by either the Autodiscover Publishing Lookup SOAP-Based Web Service Protocol,as specified by [MS-OXWSADISC], or the Autodiscover Publishing and Lookup Protocol, as specified by [MS-OXDSCLI], is required to form the HTTP request to the Web server that hosts this protocol.</t>
   </si>
   <si>
@@ -1815,9 +1812,6 @@
   </si>
   <si>
     <t>[In t:MessageType Complex Type] The MessageType complex type represents a server email message in a mailbox.</t>
-  </si>
-  <si>
-    <t>[In t:MessageType Complex Type] The MessageType complex type extends the ItemType complex type ([MS-OXWSCORE] section 2.2.4.24).</t>
   </si>
   <si>
     <t>[In t:MessageType Complex Type] The MessageType schema is &lt;xs:complexType name="MessageType"&gt;
@@ -1914,15 +1908,6 @@
     <t>[In t:MessageType Complex Type] ToRecipients element is t:ArrayOfRecipientsType ([MS-OXWSCDATA] section 2.2.4.11) type.</t>
   </si>
   <si>
-    <t>[In t:MessageType Complex Type] ToRecipients element Specifies a collection of recipients of an email.</t>
-  </si>
-  <si>
-    <t>[In t:MessageType Complex Type] BccRecipients element Specifies a collection of recipients that receive a blind carbon copy (Bcc) of an email.</t>
-  </si>
-  <si>
-    <t>[In t:MessageType Complex Type] CcRecipients element Specifies a collection of recipients that receive a carbon copy (Cc) of an email.</t>
-  </si>
-  <si>
     <t>[In t:MessageType Complex Type] ConversationIndex element is xs:base64Binary ([XMLSCHEMA2] sec 3.2.16) type.</t>
   </si>
   <si>
@@ -1941,9 +1926,6 @@
     <t>[In t:MessageType Complex Type] IsResponseRequested element Specifies a Boolean value that indicates whether a response to an email has been requested.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In t:MessageType Complex Type] ReplyTo element Specifies a collection of addresses to send replies to. </t>
-  </si>
-  <si>
     <t>[In t:MessageType Complex Type] [ReceivedBy element] This element is read-only.</t>
   </si>
   <si>
@@ -1977,9 +1959,6 @@
     <t>MS-OXWSMSG_R73002</t>
   </si>
   <si>
-    <t>MS-OXWSMSG_R73003</t>
-  </si>
-  <si>
     <t>MS-OXWSMSG_R73004</t>
   </si>
   <si>
@@ -1992,21 +1971,6 @@
     <t>MS-OXWSMSG_R73007</t>
   </si>
   <si>
-    <t>[In t:MessageDispositionType Simple Type] The value "SaveOnly" means when used in the CreateItemType complex type ([MS-OXWSCORE] section 3.1.4.2.3.2), the email message item is saved in the folder that is specified by the TargetFolderIdType complex type ([MS-OXWSFOLD] section 2.2.4.16).</t>
-  </si>
-  <si>
-    <t>[In t:MessageDispositionType Simple Type] The value "SendOnly" means when used in the CreateItemType complex type, the email message item is sent.</t>
-  </si>
-  <si>
-    <t>[In t:MessageDispositionType Simple Type] The value "SendOnly" means when used in the CreateItemType complex type, the email message item [is sent] but no copy is saved.</t>
-  </si>
-  <si>
-    <t>[In t:MessageDispositionType Simple Type] The value "SendAndSaveCopy" means when used in the CreateItemType complex type, the email message item is sent.</t>
-  </si>
-  <si>
-    <t>[In t:MessageDispositionType Simple Type] The value "SendAndSaveCopy" means when used in the CreateItemType complex type, the email message item [is sent] and a copy is saved in the TargetFolderIdType complex type.</t>
-  </si>
-  <si>
     <t>[In ExchangeServicePortType Server Details] The EMail Message Types Items Web Service Protocol defines a single port type with seven operations.</t>
   </si>
   <si>
@@ -2034,12 +1998,6 @@
     <t>[In CopyItem] The CopyItem operation copies email messages on the server.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In CopyItem] If the CreateItem WSDL operation request is successful, the server returns a CreateItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.2.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In CopyItem] [A successful CopyItem operation request returns a CopyItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element is set to "NoError". </t>
-  </si>
-  <si>
     <t xml:space="preserve">[In CopyItem] If the CreateItem WSDL operation is not successful, it returns a CreateItemResponse element with the ResponseClass attribute of the CreateItemResponseMessage element set to "Error". </t>
   </si>
   <si>
@@ -2055,12 +2013,6 @@
     <t>[In CreateItem] The CreateItem operation creates email messages.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In CreateItem]If the CreateItem WSDL operation request is successful, the server returns a CreateItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.2.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In CreateItem] [A successful CreateItem operation request returns a CreateItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element is set to "NoError". </t>
-  </si>
-  <si>
     <t xml:space="preserve">[In CreateItem] If the CreateItem WSDL operation is not successful, it returns a CreateItemResponse element with the ResponseClass attribute of the CreateItemResponseMessage element set to "Error". </t>
   </si>
   <si>
@@ -2079,12 +2031,6 @@
     <t>[In DeleteItem] The DeleteItem operation deletes email messages from the server store.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In DeleteItem] If the DeleteItem WSDL operation request is successful, the server returns a DeleteItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.3.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the DeleteItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In DeleteItem] [A successful DeleteItem operation request returns a DeleteItemResponse element] The ResponseCode element, as specified by [MS-OXWSCDATA] section 2.2.4.67, of the DeleteItemResponseMessage element is set to "NoError". </t>
-  </si>
-  <si>
     <t>[In DeleteItem] For more information, see DeleteItem as described in [MS-OXWSCORE] section 3.1.4.3.</t>
   </si>
   <si>
@@ -2103,12 +2049,6 @@
     <t>[In GetItem] The GetItem operation enables the user to get email messages and to access information about email messages.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In GetItem] If the GetItem WSDL operation request is successful, the server returns a GetItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.4.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the GetItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In GetItem] [A successful GetItem operation request returns a GetItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the GetItemResponseMessage element is set to "NoError". </t>
-  </si>
-  <si>
     <t xml:space="preserve">[In GetItem] If the GetItem WSDL operation request is not successful, it returns a GetItemResponse element with the ResponseClass attribute of the GetItemResponseMessage element set to "Error". </t>
   </si>
   <si>
@@ -2124,12 +2064,6 @@
     <t>[In MoveItem] The MoveItem operation moves one or more email messages to a single destination folder.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In MoveItem] If the MoveItem WSDL operation request is successful, the server returns a MoveItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.7.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the MoveItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In MoveItem] [A successful MoveItem operation request returns a MoveItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the MoveItemResponseMessage element is set to "NoError". </t>
-  </si>
-  <si>
     <t xml:space="preserve">[In MoveItem] If the MoveItem WSDL operation request is not successful, it returns a MoveItemResponse element with the ResponseClass attribute of the MoveItemResponseMessage element set to "Error". </t>
   </si>
   <si>
@@ -2145,12 +2079,6 @@
     <t xml:space="preserve">[In UpdateItem] The UpdateItem operation updates email message properties in the server store. </t>
   </si>
   <si>
-    <t xml:space="preserve">[In UpdateItem] If the UpdateItem WSDL operation request is successful, the server returns an UpdateItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.9.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the UpdateItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In UpdateItem] [A successful UpdateItem operation request returns an UpdateItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the UpdateItemResponseMessage element is set to "NoError". </t>
-  </si>
-  <si>
     <t xml:space="preserve">[In UpdateItem] If the UpdateItem WSDL operation request is not successful, it returns an UpdateItemResponse element with the ResponseClass attribute of the UpdateItemResponseMessage element set to "Error". </t>
   </si>
   <si>
@@ -2199,21 +2127,12 @@
     <t>MS-OXWSMSG_R73003:i</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXWSMSG_R182004.</t>
-  </si>
-  <si>
     <t>MS-OXWSMSG_R73005:i</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXWSMSG_R182006.</t>
-  </si>
-  <si>
     <t>MS-OXWSMSG_R73007:i</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXWSMSG_R182002.</t>
-  </si>
-  <si>
     <t>[In t:MessageType Complex Type] [ConversationTopic element] This element is read-only.</t>
   </si>
   <si>
@@ -2281,9 +2200,6 @@
   </si>
   <si>
     <t>[In t:ItemResponseShapeType Complex Type] otherwise [FilterHtmlContent is] false, specifies [HTML content filtering is not enabled].</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXWSMSG_R21193, MS-OXWSMSG_R21194.</t>
   </si>
   <si>
     <t>[In t:MessageType Complex Type] ReceivedBy element is t:SingleRecipientType type.</t>
@@ -2298,10 +2214,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXWSCDATA_R21188, MS-OXWSCDATA_R21189.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In t:ItemResponseShapeType Complex Type] The element "IncludeMimeContent" with type "xs:boolean" specifies whether the MIME content of an item is returned in a response.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2319,13 +2231,113 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior]&lt;53&gt; Section 2.2.4.31:  Exchange 2010 and above return the MailboxType element in the GetItem operation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageType Complex Type] ToRecipients element Specifies a collection of recipients of an email.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageDispositionType Simple Type] The value "SaveOnly" means when used in the CreateItemType complex type ([MS-OXWSCORE] section 3.1.4.2.3.2), the email message item is saved in the folder that is specified by the TargetFolderIdType complex type ([MS-OXWSFOLD] section 2.2.4.16).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageDispositionType Simple Type] The value "SendOnly" means when used in the CreateItemType complex type, the email message item [is sent] but no copy is saved.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageDispositionType Simple Type] The value "SendAndSaveCopy" means when used in the CreateItemType complex type, the email message item [is sent] and a copy is saved in the TargetFolderIdType complex type.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CopyItem] If the CreateItem WSDL operation request is successful, the server returns a CreateItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.2.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CopyItem] [A successful CopyItem operation request returns a CopyItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element is set to "NoError". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CreateItem]If the CreateItem WSDL operation request is successful, the server returns a CreateItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.2.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CreateItem] [A successful CreateItem operation request returns a CreateItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the CreateItemResponseMessage element is set to "NoError". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In DeleteItem] If the DeleteItem WSDL operation request is successful, the server returns a DeleteItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.3.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the DeleteItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In DeleteItem] [A successful DeleteItem operation request returns a DeleteItemResponse element] The ResponseCode element, as specified by [MS-OXWSCDATA] section 2.2.4.67, of the DeleteItemResponseMessage element is set to "NoError". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In GetItem] If the GetItem WSDL operation request is successful, the server returns a GetItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.4.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the GetItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In GetItem] [A successful GetItem operation request returns a GetItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the GetItemResponseMessage element is set to "NoError". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In MoveItem] [A successful MoveItem operation request returns a MoveItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the MoveItemResponseMessage element is set to "NoError". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In UpdateItem] If the UpdateItem WSDL operation request is successful, the server returns an UpdateItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.9.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the UpdateItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In UpdateItem] [A successful UpdateItem operation request returns an UpdateItemResponse element] The ResponseCode element, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the UpdateItemResponseMessage element is set to "NoError". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSMSG_R73003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXWSMSG_R2512, MS-OXWSMSG_R2912.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In MoveItem] If the MoveItem WSDL operation request is successful, the server returns a MoveItemResponse element, as specified in [MS-OXWSCORE] section 3.1.4.7.2.2, with the ResponseClass attribute, as specified in [MS-OXWSCDATA] section 2.2.4.67, of the MoveItemResponseMessage element, as specified in [MS-OXWSCDATA] section 2.2.4.12, set to "Success". </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageType Complex Type] CcRecipients element Specifies a collection of recipients that receive a carbon copy (Cc) of an email.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageType Complex Type] BccRecipients element Specifies a collection of recipients that receive a blind carbon copy (Bcc) of an email.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In t:MessageType Complex Type] ReplyTo element Specifies a collection of addresses to send replies to. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageDispositionType Simple Type] The value "SendOnly" means when used in the CreateItemType complex type, the email message item is sent.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageDispositionType Simple Type] The value "SendAndSaveCopy" means when used in the CreateItemType complex type, the email message item is sent.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Transport] This protocol uses SOAP 1.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:MessageType Complex Type] The MessageType complex type extends the ItemType complex type ([MS-OXWSCORE] section 2.2.4.24).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="0.0.0"/>
@@ -2606,21 +2618,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2639,11 +2636,528 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="113">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2980,388 +3494,6 @@
         <vertAlign val="baseline"/>
         <name val="Calibri"/>
         <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
       </font>
     </dxf>
   </dxfs>
@@ -3493,34 +3625,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I265" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I265" tableType="xml" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111" connectionId="1">
   <autoFilter ref="A19:I265"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="110">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="109">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="108">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="107">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="106">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="105">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="104">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="103">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="102">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3529,19 +3661,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98" totalsRowBorderDxfId="97">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="96"/>
+    <tableColumn id="2" name="Test" dataDxfId="95"/>
+    <tableColumn id="3" name="Description" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3830,9 +3962,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H265" sqref="H265"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3885,127 +4015,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>442</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4018,12 +4148,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -4036,12 +4166,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4054,12 +4184,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -4072,60 +4202,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>443</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -4167,7 +4297,7 @@
         <v>250</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
@@ -4192,7 +4322,7 @@
         <v>250</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -4211,13 +4341,13 @@
     </row>
     <row r="22" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="33" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>250</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D22" s="33"/>
       <c r="E22" s="33" t="s">
@@ -4236,13 +4366,13 @@
     </row>
     <row r="23" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="33" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>250</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="33" t="s">
@@ -4367,7 +4497,7 @@
         <v>252</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>444</v>
+        <v>588</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -4417,7 +4547,7 @@
         <v>252</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -4436,13 +4566,13 @@
     </row>
     <row r="31" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>252</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="33" t="s">
@@ -4519,7 +4649,7 @@
         <v>253</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22" t="s">
@@ -4819,7 +4949,7 @@
         <v>257</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30" t="s">
@@ -4844,7 +4974,7 @@
         <v>31</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30" t="s">
@@ -4869,7 +4999,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>457</v>
+        <v>589</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30" t="s">
@@ -4894,7 +5024,7 @@
         <v>31</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30" t="s">
@@ -4944,7 +5074,7 @@
         <v>31</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30" t="s">
@@ -5098,7 +5228,7 @@
         <v>31</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D57" s="30"/>
       <c r="E57" s="30" t="s">
@@ -5177,7 +5307,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>461</v>
+        <v>565</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -5277,7 +5407,7 @@
         <v>31</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>463</v>
+        <v>583</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30" t="s">
@@ -5377,7 +5507,7 @@
         <v>31</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>462</v>
+        <v>584</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="s">
@@ -5452,7 +5582,7 @@
         <v>31</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>574</v>
+        <v>547</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30" t="s">
@@ -5731,7 +5861,7 @@
         <v>31</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30" t="s">
@@ -5756,7 +5886,7 @@
         <v>31</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="30" t="s">
@@ -5806,7 +5936,7 @@
         <v>31</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D85" s="30"/>
       <c r="E85" s="30" t="s">
@@ -5831,7 +5961,7 @@
         <v>31</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>575</v>
+        <v>548</v>
       </c>
       <c r="D86" s="30"/>
       <c r="E86" s="30" t="s">
@@ -5906,7 +6036,7 @@
         <v>31</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>561</v>
+        <v>534</v>
       </c>
       <c r="D89" s="30"/>
       <c r="E89" s="30" t="s">
@@ -6106,7 +6236,7 @@
         <v>31</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D97" s="30"/>
       <c r="E97" s="30" t="s">
@@ -6181,7 +6311,7 @@
         <v>31</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="30" t="s">
@@ -6283,7 +6413,7 @@
         <v>31</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="30" t="s">
@@ -6535,7 +6665,7 @@
         <v>31</v>
       </c>
       <c r="C114" s="20" t="s">
-        <v>470</v>
+        <v>585</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30" t="s">
@@ -6610,7 +6740,7 @@
         <v>31</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
@@ -6654,13 +6784,13 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="22" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B119" s="24" t="s">
         <v>31</v>
       </c>
       <c r="C119" s="35" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D119" s="33"/>
       <c r="E119" s="33" t="s">
@@ -6729,13 +6859,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="22" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C122" s="35" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D122" s="33"/>
       <c r="E122" s="33" t="s">
@@ -6754,13 +6884,13 @@
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="22" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C123" s="35" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D123" s="33"/>
       <c r="E123" s="33" t="s">
@@ -6779,13 +6909,13 @@
     </row>
     <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="22" t="s">
-        <v>482</v>
+        <v>580</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C124" s="35" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="D124" s="33"/>
       <c r="E124" s="33" t="s">
@@ -6800,19 +6930,17 @@
       <c r="H124" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I124" s="35" t="s">
-        <v>560</v>
-      </c>
+      <c r="I124" s="35"/>
     </row>
     <row r="125" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="22" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C125" s="35" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D125" s="33"/>
       <c r="E125" s="33" t="s">
@@ -6831,13 +6959,13 @@
     </row>
     <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C126" s="35" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="D126" s="33"/>
       <c r="E126" s="33" t="s">
@@ -6852,19 +6980,17 @@
       <c r="H126" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I126" s="35" t="s">
-        <v>556</v>
-      </c>
+      <c r="I126" s="35"/>
     </row>
     <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C127" s="35" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="D127" s="33"/>
       <c r="E127" s="33" t="s">
@@ -6881,15 +7007,15 @@
       </c>
       <c r="I127" s="35"/>
     </row>
-    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="22" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="B128" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C128" s="35" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D128" s="33"/>
       <c r="E128" s="33" t="s">
@@ -6904,9 +7030,7 @@
       <c r="H128" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I128" s="35" t="s">
-        <v>558</v>
-      </c>
+      <c r="I128" s="35"/>
     </row>
     <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="30" t="s">
@@ -7066,7 +7190,7 @@
         <v>259</v>
       </c>
       <c r="C135" s="20" t="s">
-        <v>487</v>
+        <v>566</v>
       </c>
       <c r="D135" s="30"/>
       <c r="E135" s="30" t="s">
@@ -7141,7 +7265,7 @@
         <v>259</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>488</v>
+        <v>586</v>
       </c>
       <c r="D138" s="30"/>
       <c r="E138" s="30" t="s">
@@ -7166,7 +7290,7 @@
         <v>259</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>489</v>
+        <v>567</v>
       </c>
       <c r="D139" s="30"/>
       <c r="E139" s="30" t="s">
@@ -7216,7 +7340,7 @@
         <v>259</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>490</v>
+        <v>587</v>
       </c>
       <c r="D141" s="30"/>
       <c r="E141" s="30" t="s">
@@ -7241,7 +7365,7 @@
         <v>259</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>491</v>
+        <v>568</v>
       </c>
       <c r="D142" s="30"/>
       <c r="E142" s="30" t="s">
@@ -7441,7 +7565,7 @@
         <v>264</v>
       </c>
       <c r="C150" s="20" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="D150" s="30"/>
       <c r="E150" s="30" t="s">
@@ -7591,7 +7715,7 @@
         <v>266</v>
       </c>
       <c r="C156" s="20" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="D156" s="30"/>
       <c r="E156" s="30" t="s">
@@ -7616,7 +7740,7 @@
         <v>266</v>
       </c>
       <c r="C157" s="20" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="D157" s="30"/>
       <c r="E157" s="30" t="s">
@@ -7641,7 +7765,7 @@
         <v>266</v>
       </c>
       <c r="C158" s="20" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="D158" s="30"/>
       <c r="E158" s="30" t="s">
@@ -7666,7 +7790,7 @@
         <v>266</v>
       </c>
       <c r="C159" s="20" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="D159" s="30"/>
       <c r="E159" s="30" t="s">
@@ -7691,7 +7815,7 @@
         <v>266</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="D160" s="30"/>
       <c r="E160" s="30" t="s">
@@ -7716,7 +7840,7 @@
         <v>266</v>
       </c>
       <c r="C161" s="20" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="D161" s="30"/>
       <c r="E161" s="30" t="s">
@@ -7741,7 +7865,7 @@
         <v>266</v>
       </c>
       <c r="C162" s="20" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="D162" s="30"/>
       <c r="E162" s="30" t="s">
@@ -7766,7 +7890,7 @@
         <v>32</v>
       </c>
       <c r="C163" s="20" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="D163" s="30"/>
       <c r="E163" s="30" t="s">
@@ -7866,7 +7990,7 @@
         <v>32</v>
       </c>
       <c r="C167" s="20" t="s">
-        <v>501</v>
+        <v>569</v>
       </c>
       <c r="D167" s="30"/>
       <c r="E167" s="30" t="s">
@@ -7891,7 +8015,7 @@
         <v>32</v>
       </c>
       <c r="C168" s="20" t="s">
-        <v>502</v>
+        <v>570</v>
       </c>
       <c r="D168" s="30"/>
       <c r="E168" s="30" t="s">
@@ -7910,13 +8034,13 @@
     </row>
     <row r="169" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="22" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="B169" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C169" s="35" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="D169" s="33"/>
       <c r="E169" s="33" t="s">
@@ -7935,13 +8059,13 @@
     </row>
     <row r="170" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="22" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="B170" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C170" s="35" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
       <c r="D170" s="33"/>
       <c r="E170" s="33" t="s">
@@ -7966,7 +8090,7 @@
         <v>32</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="D171" s="30"/>
       <c r="E171" s="30" t="s">
@@ -7991,7 +8115,7 @@
         <v>33</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="D172" s="30"/>
       <c r="E172" s="30" t="s">
@@ -8091,7 +8215,7 @@
         <v>33</v>
       </c>
       <c r="C176" s="20" t="s">
-        <v>508</v>
+        <v>571</v>
       </c>
       <c r="D176" s="30"/>
       <c r="E176" s="30" t="s">
@@ -8116,7 +8240,7 @@
         <v>33</v>
       </c>
       <c r="C177" s="20" t="s">
-        <v>509</v>
+        <v>572</v>
       </c>
       <c r="D177" s="30"/>
       <c r="E177" s="30" t="s">
@@ -8135,13 +8259,13 @@
     </row>
     <row r="178" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="22" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="B178" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C178" s="35" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="D178" s="33"/>
       <c r="E178" s="33" t="s">
@@ -8160,13 +8284,13 @@
     </row>
     <row r="179" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="B179" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C179" s="35" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
       <c r="D179" s="33"/>
       <c r="E179" s="33" t="s">
@@ -8216,7 +8340,7 @@
         <v>267</v>
       </c>
       <c r="C181" s="20" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
       <c r="D181" s="30"/>
       <c r="E181" s="30" t="s">
@@ -8316,7 +8440,7 @@
         <v>267</v>
       </c>
       <c r="C185" s="20" t="s">
-        <v>516</v>
+        <v>573</v>
       </c>
       <c r="D185" s="30"/>
       <c r="E185" s="30" t="s">
@@ -8341,7 +8465,7 @@
         <v>267</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>517</v>
+        <v>574</v>
       </c>
       <c r="D186" s="30"/>
       <c r="E186" s="30" t="s">
@@ -8360,13 +8484,13 @@
     </row>
     <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="22" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="B187" s="24" t="s">
         <v>267</v>
       </c>
       <c r="C187" s="35" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="D187" s="33"/>
       <c r="E187" s="30" t="s">
@@ -8385,13 +8509,13 @@
     </row>
     <row r="188" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="22" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="B188" s="24" t="s">
         <v>267</v>
       </c>
       <c r="C188" s="35" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
       <c r="D188" s="33"/>
       <c r="E188" s="30" t="s">
@@ -8416,7 +8540,7 @@
         <v>267</v>
       </c>
       <c r="C189" s="20" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="D189" s="30"/>
       <c r="E189" s="30" t="s">
@@ -8441,7 +8565,7 @@
         <v>268</v>
       </c>
       <c r="C190" s="20" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
       <c r="D190" s="30"/>
       <c r="E190" s="30" t="s">
@@ -8782,7 +8906,7 @@
         <v>17</v>
       </c>
       <c r="I203" s="20" t="s">
-        <v>562</v>
+        <v>535</v>
       </c>
     </row>
     <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8809,7 +8933,7 @@
         <v>17</v>
       </c>
       <c r="I204" s="20" t="s">
-        <v>568</v>
+        <v>541</v>
       </c>
     </row>
     <row r="205" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8836,7 +8960,7 @@
         <v>17</v>
       </c>
       <c r="I205" s="20" t="s">
-        <v>576</v>
+        <v>549</v>
       </c>
     </row>
     <row r="206" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8863,7 +8987,7 @@
         <v>17</v>
       </c>
       <c r="I206" s="20" t="s">
-        <v>571</v>
+        <v>544</v>
       </c>
     </row>
     <row r="207" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8899,7 +9023,7 @@
         <v>268</v>
       </c>
       <c r="C208" s="20" t="s">
-        <v>524</v>
+        <v>575</v>
       </c>
       <c r="D208" s="30"/>
       <c r="E208" s="30" t="s">
@@ -8924,7 +9048,7 @@
         <v>268</v>
       </c>
       <c r="C209" s="20" t="s">
-        <v>525</v>
+        <v>576</v>
       </c>
       <c r="D209" s="30"/>
       <c r="E209" s="30" t="s">
@@ -8943,13 +9067,13 @@
     </row>
     <row r="210" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="22" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="B210" s="24" t="s">
         <v>268</v>
       </c>
       <c r="C210" s="35" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
       <c r="D210" s="33"/>
       <c r="E210" s="30" t="s">
@@ -8968,13 +9092,13 @@
     </row>
     <row r="211" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="22" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="B211" s="24" t="s">
         <v>268</v>
       </c>
       <c r="C211" s="35" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="D211" s="33"/>
       <c r="E211" s="30" t="s">
@@ -9024,7 +9148,7 @@
         <v>269</v>
       </c>
       <c r="C213" s="20" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="D213" s="30"/>
       <c r="E213" s="30" t="s">
@@ -9124,7 +9248,7 @@
         <v>269</v>
       </c>
       <c r="C217" s="20" t="s">
-        <v>531</v>
+        <v>582</v>
       </c>
       <c r="D217" s="30"/>
       <c r="E217" s="30" t="s">
@@ -9149,7 +9273,7 @@
         <v>269</v>
       </c>
       <c r="C218" s="20" t="s">
-        <v>532</v>
+        <v>577</v>
       </c>
       <c r="D218" s="30"/>
       <c r="E218" s="30" t="s">
@@ -9168,13 +9292,13 @@
     </row>
     <row r="219" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="22" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="B219" s="31" t="s">
         <v>269</v>
       </c>
       <c r="C219" s="35" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
       <c r="D219" s="33"/>
       <c r="E219" s="30" t="s">
@@ -9193,13 +9317,13 @@
     </row>
     <row r="220" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="22" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="B220" s="31" t="s">
         <v>269</v>
       </c>
       <c r="C220" s="35" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="D220" s="33"/>
       <c r="E220" s="30" t="s">
@@ -9424,7 +9548,7 @@
         <v>271</v>
       </c>
       <c r="C229" s="20" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
       <c r="D229" s="30"/>
       <c r="E229" s="30" t="s">
@@ -9599,7 +9723,7 @@
         <v>271</v>
       </c>
       <c r="C236" s="20" t="s">
-        <v>538</v>
+        <v>578</v>
       </c>
       <c r="D236" s="30"/>
       <c r="E236" s="30" t="s">
@@ -9624,7 +9748,7 @@
         <v>271</v>
       </c>
       <c r="C237" s="20" t="s">
-        <v>539</v>
+        <v>579</v>
       </c>
       <c r="D237" s="30"/>
       <c r="E237" s="30" t="s">
@@ -9643,13 +9767,13 @@
     </row>
     <row r="238" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" s="22" t="s">
-        <v>542</v>
+        <v>518</v>
       </c>
       <c r="B238" s="24" t="s">
         <v>271</v>
       </c>
       <c r="C238" s="35" t="s">
-        <v>540</v>
+        <v>516</v>
       </c>
       <c r="D238" s="33"/>
       <c r="E238" s="30" t="s">
@@ -9668,13 +9792,13 @@
     </row>
     <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="22" t="s">
-        <v>543</v>
+        <v>519</v>
       </c>
       <c r="B239" s="24" t="s">
         <v>271</v>
       </c>
       <c r="C239" s="35" t="s">
-        <v>541</v>
+        <v>517</v>
       </c>
       <c r="D239" s="33"/>
       <c r="E239" s="30" t="s">
@@ -9716,7 +9840,7 @@
       </c>
       <c r="I240" s="32"/>
     </row>
-    <row r="241" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="30" t="s">
         <v>240</v>
       </c>
@@ -9741,7 +9865,7 @@
       </c>
       <c r="I241" s="32"/>
     </row>
-    <row r="242" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="30" t="s">
         <v>241</v>
       </c>
@@ -9770,7 +9894,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="30" t="s">
         <v>242</v>
       </c>
@@ -9795,18 +9919,18 @@
       </c>
       <c r="I243" s="32"/>
     </row>
-    <row r="244" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A244" s="22" t="s">
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="B244" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C244" s="35" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
       <c r="D244" s="33" t="s">
-        <v>555</v>
+        <v>531</v>
       </c>
       <c r="E244" s="30" t="s">
         <v>22</v>
@@ -9822,18 +9946,18 @@
       </c>
       <c r="I244" s="35"/>
     </row>
-    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="22" t="s">
-        <v>550</v>
+        <v>526</v>
       </c>
       <c r="B245" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C245" s="35" t="s">
-        <v>545</v>
+        <v>521</v>
       </c>
       <c r="D245" s="33" t="s">
-        <v>555</v>
+        <v>531</v>
       </c>
       <c r="E245" s="30" t="s">
         <v>22</v>
@@ -9847,20 +9971,22 @@
       <c r="H245" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I245" s="35"/>
-    </row>
-    <row r="246" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I245" s="32" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="22" t="s">
-        <v>551</v>
+        <v>527</v>
       </c>
       <c r="B246" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C246" s="35" t="s">
-        <v>592</v>
+        <v>563</v>
       </c>
       <c r="D246" s="33" t="s">
-        <v>557</v>
+        <v>532</v>
       </c>
       <c r="E246" s="30" t="s">
         <v>22</v>
@@ -9876,18 +10002,18 @@
       </c>
       <c r="I246" s="35"/>
     </row>
-    <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A247" s="22" t="s">
-        <v>552</v>
+        <v>528</v>
       </c>
       <c r="B247" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C247" s="35" t="s">
-        <v>548</v>
+        <v>524</v>
       </c>
       <c r="D247" s="33" t="s">
-        <v>557</v>
+        <v>532</v>
       </c>
       <c r="E247" s="30" t="s">
         <v>22</v>
@@ -9901,20 +10027,22 @@
       <c r="H247" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I247" s="35"/>
-    </row>
-    <row r="248" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I247" s="32" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A248" s="22" t="s">
-        <v>553</v>
+        <v>529</v>
       </c>
       <c r="B248" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C248" s="35" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="D248" s="33" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="E248" s="30" t="s">
         <v>22</v>
@@ -9930,18 +10058,18 @@
       </c>
       <c r="I248" s="35"/>
     </row>
-    <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A249" s="22" t="s">
-        <v>554</v>
+        <v>530</v>
       </c>
       <c r="B249" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C249" s="35" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
       <c r="D249" s="33" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="E249" s="30" t="s">
         <v>22</v>
@@ -9955,9 +10083,11 @@
       <c r="H249" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I249" s="35"/>
-    </row>
-    <row r="250" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="I249" s="32" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A250" s="30" t="s">
         <v>243</v>
       </c>
@@ -9982,7 +10112,7 @@
       </c>
       <c r="I250" s="32"/>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" s="30" t="s">
         <v>244</v>
       </c>
@@ -10005,9 +10135,11 @@
       <c r="H251" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I251" s="32"/>
-    </row>
-    <row r="252" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I251" s="20" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A252" s="30" t="s">
         <v>245</v>
       </c>
@@ -10034,7 +10166,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A253" s="30" t="s">
         <v>246</v>
       </c>
@@ -10059,90 +10191,97 @@
       </c>
       <c r="I253" s="32"/>
     </row>
-    <row r="254" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A254" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="B254" s="31" t="s">
-        <v>275</v>
-      </c>
-      <c r="C254" s="32" t="s">
-        <v>424</v>
-      </c>
-      <c r="D254" s="30"/>
-      <c r="E254" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F254" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G254" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H254" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I254" s="32"/>
-    </row>
-    <row r="255" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A255" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B255" s="31" t="s">
-        <v>276</v>
-      </c>
-      <c r="C255" s="32" t="s">
-        <v>425</v>
-      </c>
-      <c r="D255" s="30"/>
-      <c r="E255" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F255" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G255" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H255" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I255" s="32"/>
-    </row>
-    <row r="256" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A256" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="B256" s="31" t="s">
-        <v>277</v>
-      </c>
-      <c r="C256" s="32" t="s">
-        <v>426</v>
-      </c>
-      <c r="D256" s="30"/>
-      <c r="E256" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F256" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G256" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H256" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I256" s="32"/>
+    <row r="254" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A254" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="B254" s="24" t="s">
+        <v>537</v>
+      </c>
+      <c r="C254" s="20" t="s">
+        <v>560</v>
+      </c>
+      <c r="D254" s="22"/>
+      <c r="E254" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F254" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G254" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H254" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I254" s="20"/>
+      <c r="J254"/>
+    </row>
+    <row r="255" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A255" s="22" t="s">
+        <v>558</v>
+      </c>
+      <c r="B255" s="24" t="s">
+        <v>537</v>
+      </c>
+      <c r="C255" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="D255" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="E255" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F255" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G255" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H255" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I255" s="20"/>
+      <c r="J255"/>
+    </row>
+    <row r="256" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A256" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="B256" s="24" t="s">
+        <v>537</v>
+      </c>
+      <c r="C256" s="20" t="s">
+        <v>540</v>
+      </c>
+      <c r="D256" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="E256" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F256" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G256" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H256" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I256" s="20"/>
+      <c r="J256"/>
     </row>
     <row r="257" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="22" t="s">
-        <v>563</v>
+        <v>542</v>
       </c>
       <c r="B257" s="24" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="C257" s="20" t="s">
-        <v>589</v>
+        <v>543</v>
       </c>
       <c r="D257" s="22"/>
       <c r="E257" s="22" t="s">
@@ -10155,26 +10294,22 @@
         <v>15</v>
       </c>
       <c r="H257" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I257" s="20" t="s">
-        <v>588</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I257" s="20"/>
       <c r="J257"/>
     </row>
-    <row r="258" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A258" s="22" t="s">
-        <v>586</v>
+        <v>545</v>
       </c>
       <c r="B258" s="24" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="C258" s="20" t="s">
-        <v>565</v>
-      </c>
-      <c r="D258" s="22" t="s">
-        <v>566</v>
-      </c>
+        <v>546</v>
+      </c>
+      <c r="D258" s="22"/>
       <c r="E258" s="22" t="s">
         <v>19</v>
       </c>
@@ -10192,17 +10327,15 @@
     </row>
     <row r="259" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="22" t="s">
-        <v>587</v>
+        <v>550</v>
       </c>
       <c r="B259" s="24" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="C259" s="20" t="s">
-        <v>567</v>
-      </c>
-      <c r="D259" s="22" t="s">
-        <v>566</v>
-      </c>
+        <v>551</v>
+      </c>
+      <c r="D259" s="22"/>
       <c r="E259" s="22" t="s">
         <v>19</v>
       </c>
@@ -10218,17 +10351,19 @@
       <c r="I259" s="20"/>
       <c r="J259"/>
     </row>
-    <row r="260" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="22" t="s">
-        <v>569</v>
+        <v>552</v>
       </c>
       <c r="B260" s="24" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="C260" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="D260" s="22"/>
+        <v>553</v>
+      </c>
+      <c r="D260" s="22" t="s">
+        <v>554</v>
+      </c>
       <c r="E260" s="22" t="s">
         <v>19</v>
       </c>
@@ -10244,17 +10379,19 @@
       <c r="I260" s="20"/>
       <c r="J260"/>
     </row>
-    <row r="261" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="22" t="s">
-        <v>572</v>
+        <v>555</v>
       </c>
       <c r="B261" s="24" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="C261" s="20" t="s">
-        <v>573</v>
-      </c>
-      <c r="D261" s="22"/>
+        <v>556</v>
+      </c>
+      <c r="D261" s="22" t="s">
+        <v>554</v>
+      </c>
       <c r="E261" s="22" t="s">
         <v>19</v>
       </c>
@@ -10270,103 +10407,94 @@
       <c r="I261" s="20"/>
       <c r="J261"/>
     </row>
-    <row r="262" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A262" s="22" t="s">
-        <v>579</v>
-      </c>
-      <c r="B262" s="24" t="s">
-        <v>564</v>
-      </c>
-      <c r="C262" s="20" t="s">
-        <v>580</v>
-      </c>
-      <c r="D262" s="22" t="s">
-        <v>581</v>
-      </c>
-      <c r="E262" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F262" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G262" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H262" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I262" s="20"/>
-      <c r="J262"/>
-    </row>
-    <row r="263" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A263" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="B263" s="24" t="s">
-        <v>564</v>
-      </c>
-      <c r="C263" s="20" t="s">
-        <v>583</v>
-      </c>
-      <c r="D263" s="22" t="s">
-        <v>581</v>
-      </c>
-      <c r="E263" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F263" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G263" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H263" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I263" s="20"/>
-      <c r="J263"/>
-    </row>
-    <row r="264" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A264" s="22" t="s">
-        <v>577</v>
-      </c>
-      <c r="B264" s="24" t="s">
-        <v>564</v>
-      </c>
-      <c r="C264" s="20" t="s">
-        <v>578</v>
-      </c>
-      <c r="D264" s="22"/>
-      <c r="E264" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F264" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G264" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H264" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I264" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="J264"/>
+    <row r="262" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A262" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="B262" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="C262" s="32" t="s">
+        <v>424</v>
+      </c>
+      <c r="D262" s="30"/>
+      <c r="E262" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F262" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G262" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H262" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I262" s="32"/>
+    </row>
+    <row r="263" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A263" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="B263" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="C263" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="D263" s="30"/>
+      <c r="E263" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F263" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G263" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H263" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I263" s="32"/>
+    </row>
+    <row r="264" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A264" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="B264" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="C264" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="D264" s="30"/>
+      <c r="E264" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F264" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G264" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H264" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I264" s="32"/>
     </row>
     <row r="265" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A265" s="22" t="s">
-        <v>590</v>
+        <v>561</v>
       </c>
       <c r="B265" s="24" t="s">
-        <v>591</v>
+        <v>562</v>
       </c>
       <c r="C265" s="20" t="s">
-        <v>593</v>
+        <v>564</v>
       </c>
       <c r="D265" s="22"/>
-      <c r="E265" s="22" t="s">
-        <v>19</v>
+      <c r="E265" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="F265" s="22" t="s">
         <v>3</v>
@@ -10388,6 +10516,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -10395,272 +10528,355 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:I255 A262:I263">
-    <cfRule type="expression" dxfId="88" priority="139">
+  <conditionalFormatting sqref="A260:I263 A252:I253 A251:H251 A20:I250">
+    <cfRule type="expression" dxfId="93" priority="163">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="140">
+    <cfRule type="expression" dxfId="92" priority="164">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="147">
+    <cfRule type="expression" dxfId="91" priority="171">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:I255 A262:I263">
-    <cfRule type="expression" dxfId="85" priority="93">
+  <conditionalFormatting sqref="A260:I263 A252:I253 A251:H251 A20:I250">
+    <cfRule type="expression" dxfId="90" priority="117">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="94">
+    <cfRule type="expression" dxfId="89" priority="118">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="95">
+    <cfRule type="expression" dxfId="88" priority="119">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F255 F262:F263">
-    <cfRule type="expression" dxfId="82" priority="99">
+  <conditionalFormatting sqref="F20:F253 F260:F263">
+    <cfRule type="expression" dxfId="87" priority="123">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="100">
+    <cfRule type="expression" dxfId="86" priority="124">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A260:I260">
-    <cfRule type="expression" dxfId="80" priority="44">
+  <conditionalFormatting sqref="A257:I257">
+    <cfRule type="expression" dxfId="85" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="45">
+    <cfRule type="expression" dxfId="84" priority="69">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="46">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A260:I260">
-    <cfRule type="expression" dxfId="77" priority="39">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="40">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="41">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F260">
-    <cfRule type="expression" dxfId="74" priority="42">
-      <formula>NOT(VLOOKUP(F260,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="43">
-      <formula>(VLOOKUP(F260,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A256:I256">
-    <cfRule type="expression" dxfId="72" priority="76">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="77">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="78">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A256:I256">
-    <cfRule type="expression" dxfId="69" priority="71">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="72">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="73">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F256">
-    <cfRule type="expression" dxfId="66" priority="74">
-      <formula>NOT(VLOOKUP(F256,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="75">
-      <formula>(VLOOKUP(F256,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A257:I257">
-    <cfRule type="expression" dxfId="64" priority="60">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="61">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="62">
+    <cfRule type="expression" dxfId="83" priority="70">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A257:I257">
-    <cfRule type="expression" dxfId="61" priority="55">
+    <cfRule type="expression" dxfId="82" priority="63">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="56">
+    <cfRule type="expression" dxfId="81" priority="64">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="57">
+    <cfRule type="expression" dxfId="80" priority="65">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F257">
-    <cfRule type="expression" dxfId="58" priority="58">
+    <cfRule type="expression" dxfId="79" priority="66">
       <formula>NOT(VLOOKUP(F257,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="59">
+    <cfRule type="expression" dxfId="78" priority="67">
       <formula>(VLOOKUP(F257,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A258:I259">
-    <cfRule type="expression" dxfId="56" priority="52">
+  <conditionalFormatting sqref="A264:I264">
+    <cfRule type="expression" dxfId="77" priority="100">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="53">
+    <cfRule type="expression" dxfId="76" priority="101">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="54">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A258:I259">
-    <cfRule type="expression" dxfId="53" priority="47">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="48">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="49">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F258:F259">
-    <cfRule type="expression" dxfId="50" priority="50">
-      <formula>NOT(VLOOKUP(F258,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="51">
-      <formula>(VLOOKUP(F258,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A261:I261">
-    <cfRule type="expression" dxfId="48" priority="36">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="37">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="38">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A261:I261">
-    <cfRule type="expression" dxfId="45" priority="31">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="32">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="33">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F261">
-    <cfRule type="expression" dxfId="42" priority="34">
-      <formula>NOT(VLOOKUP(F261,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="35">
-      <formula>(VLOOKUP(F261,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A264:I264">
-    <cfRule type="expression" dxfId="40" priority="20">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="21">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="75" priority="102">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:I264">
-    <cfRule type="expression" dxfId="37" priority="15">
+    <cfRule type="expression" dxfId="74" priority="95">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="73" priority="96">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="17">
+    <cfRule type="expression" dxfId="72" priority="97">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F264">
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="71" priority="98">
       <formula>NOT(VLOOKUP(F264,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="19">
+    <cfRule type="expression" dxfId="70" priority="99">
       <formula>(VLOOKUP(F264,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A265:H265">
-    <cfRule type="expression" dxfId="32" priority="12">
+  <conditionalFormatting sqref="A254:G254 I254">
+    <cfRule type="expression" dxfId="69" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="13">
+    <cfRule type="expression" dxfId="68" priority="85">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="67" priority="86">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A265:H265">
-    <cfRule type="expression" dxfId="29" priority="7">
+  <conditionalFormatting sqref="A254:G254 I254">
+    <cfRule type="expression" dxfId="66" priority="79">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="65" priority="80">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9">
+    <cfRule type="expression" dxfId="64" priority="81">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F254">
+    <cfRule type="expression" dxfId="63" priority="82">
+      <formula>NOT(VLOOKUP(F254,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="83">
+      <formula>(VLOOKUP(F254,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A255:I256">
+    <cfRule type="expression" dxfId="61" priority="76">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="77">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="78">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A255:I256">
+    <cfRule type="expression" dxfId="58" priority="71">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="72">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="73">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F255:F256">
+    <cfRule type="expression" dxfId="55" priority="74">
+      <formula>NOT(VLOOKUP(F255,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="75">
+      <formula>(VLOOKUP(F255,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A258:I258">
+    <cfRule type="expression" dxfId="53" priority="60">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="61">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="62">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A258:I258">
+    <cfRule type="expression" dxfId="50" priority="55">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="56">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="57">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F258">
+    <cfRule type="expression" dxfId="47" priority="58">
+      <formula>NOT(VLOOKUP(F258,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="59">
+      <formula>(VLOOKUP(F258,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A259:G259 I259">
+    <cfRule type="expression" dxfId="45" priority="44">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="45">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="46">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A259:G259 I259">
+    <cfRule type="expression" dxfId="42" priority="39">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="40">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="41">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F259">
+    <cfRule type="expression" dxfId="39" priority="42">
+      <formula>NOT(VLOOKUP(F259,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="43">
+      <formula>(VLOOKUP(F259,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A265:D265 F265:H265">
+    <cfRule type="expression" dxfId="37" priority="36">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="37">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="38">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A265:D265 F265:H265">
+    <cfRule type="expression" dxfId="34" priority="31">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="32">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="33">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F265">
-    <cfRule type="expression" dxfId="26" priority="10">
+    <cfRule type="expression" dxfId="31" priority="34">
       <formula>NOT(VLOOKUP(F265,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="11">
+    <cfRule type="expression" dxfId="30" priority="35">
       <formula>(VLOOKUP(F265,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I265">
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="29" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="28" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="27" priority="30">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I265">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="26" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="24" priority="27">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H254">
+    <cfRule type="expression" dxfId="23" priority="22">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="24">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H254">
+    <cfRule type="expression" dxfId="20" priority="19">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="21">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H259">
+    <cfRule type="expression" dxfId="17" priority="16">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H259">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E265">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E265">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I251">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I251">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10678,10 +10894,10 @@
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H256">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H253 H262:H264">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H257:H265">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H265 H254:H261">
       <formula1>"Message Deserialization, Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10691,7 +10907,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 C3 B11:B16 B18:B21 B24:B30 B32:B118 B120:B121 B129:B162 B241:B243 B266 B250:B255" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 C3 B11:B16 B18:B21 B24:B30 B32:B118 B120:B121 B129:B162 B241:B243 B266 B262:B263 B250:B253" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -10701,6 +10917,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -10749,12 +10971,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10765,6 +10981,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10779,20 +11009,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[MS-OXWSMSG] fix watchman error
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="593">
   <si>
     <t>Req ID</t>
   </si>
@@ -2188,9 +2188,6 @@
     <t>[In t:ItemResponseShapeType Complex Type] otherwise [FilterHtmlContent is] false, specifies [HTML content filtering is not enabled].</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXWSMSG_R21193, MS-OXWSMSG_R21194.</t>
-  </si>
-  <si>
     <t>[In t:MessageType Complex Type] ReceivedBy element is t:SingleRecipientType type.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2203,15 +2200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXWSCDATA_R21188, MS-OXWSCDATA_R21189.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In t:ItemResponseShapeType Complex Type] The element "IncludeMimeContent" with type "xs:boolean" specifies whether the MIME content of an item is returned in a response.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS-OXWSCDATA_R1428001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2331,6 +2320,9 @@
   </si>
   <si>
     <t>Verified by derived requirements: MS-OXWSMSG_R2512, MS-OXWSMSG_R2912</t>
+  </si>
+  <si>
+    <t>MS-OXWSCDATA_R1428001</t>
   </si>
 </sst>
 </file>
@@ -2617,21 +2609,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2655,6 +2632,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3633,6 +3625,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3668,6 +3677,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3900,127 +3926,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="75.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="30.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>442</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -4033,12 +4059,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
@@ -4051,12 +4077,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -4069,12 +4095,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -4087,60 +4113,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="61.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
-        <v>590</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="B17" s="42" t="s">
+        <v>587</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -6625,7 +6651,7 @@
         <v>31</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
@@ -6816,7 +6842,7 @@
         <v>17</v>
       </c>
       <c r="I124" s="20" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="30">
@@ -6868,7 +6894,7 @@
         <v>17</v>
       </c>
       <c r="I126" s="20" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="30">
@@ -6920,7 +6946,7 @@
         <v>17</v>
       </c>
       <c r="I128" s="20" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="30">
@@ -9872,7 +9898,7 @@
         <v>272</v>
       </c>
       <c r="C246" s="35" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D246" s="33" t="s">
         <v>555</v>
@@ -10021,7 +10047,7 @@
         <v>17</v>
       </c>
       <c r="I251" s="20" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="252" spans="1:10" ht="60">
@@ -10126,7 +10152,7 @@
       </c>
       <c r="I255" s="32"/>
     </row>
-    <row r="256" spans="1:10" ht="60">
+    <row r="256" spans="1:10" ht="30">
       <c r="A256" s="22" t="s">
         <v>559</v>
       </c>
@@ -10134,7 +10160,7 @@
         <v>560</v>
       </c>
       <c r="C256" s="20" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D256" s="22"/>
       <c r="E256" s="22" t="s">
@@ -10149,14 +10175,12 @@
       <c r="H256" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I256" s="20" t="s">
-        <v>584</v>
-      </c>
+      <c r="I256" s="20"/>
       <c r="J256"/>
     </row>
     <row r="257" spans="1:10" ht="30">
       <c r="A257" s="22" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B257" s="24" t="s">
         <v>560</v>
@@ -10184,7 +10208,7 @@
     </row>
     <row r="258" spans="1:10" ht="30">
       <c r="A258" s="22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B258" s="24" t="s">
         <v>560</v>
@@ -10318,7 +10342,7 @@
       <c r="I262" s="20"/>
       <c r="J262"/>
     </row>
-    <row r="263" spans="1:10" ht="60">
+    <row r="263" spans="1:10" ht="30">
       <c r="A263" s="22" t="s">
         <v>573</v>
       </c>
@@ -10341,9 +10365,7 @@
       <c r="H263" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I263" s="20" t="s">
-        <v>580</v>
-      </c>
+      <c r="I263" s="20"/>
       <c r="J263"/>
     </row>
     <row r="264" spans="1:10" ht="135">
@@ -10373,17 +10395,17 @@
     </row>
     <row r="265" spans="1:10" ht="45">
       <c r="A265" s="22" t="s">
+        <v>592</v>
+      </c>
+      <c r="B265" s="24" t="s">
+        <v>584</v>
+      </c>
+      <c r="C265" s="20" t="s">
         <v>586</v>
-      </c>
-      <c r="B265" s="24" t="s">
-        <v>587</v>
-      </c>
-      <c r="C265" s="20" t="s">
-        <v>589</v>
       </c>
       <c r="D265" s="22"/>
       <c r="E265" s="22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F265" s="22" t="s">
         <v>3</v>
@@ -10405,6 +10427,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -10412,11 +10439,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I165 A261:I262 A167:I255 A166:H166">

</xml_diff>

<commit_message>
update RS of MS-OXWSMSG
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC4E17-26C6-488D-99C8-838D22864EF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EABAA239-24BB-46BA-8BFD-ED43F6928875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="778">
   <si>
     <t>Req ID</t>
   </si>
@@ -2910,6 +2910,9 @@
   </si>
   <si>
     <t>MS-OXWSMSG_R73010</t>
+  </si>
+  <si>
+    <t>MS-OXWSMSG_R444</t>
   </si>
 </sst>
 </file>
@@ -3214,21 +3217,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3253,12 +3241,365 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="89">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -3641,344 +3982,6 @@
         <strike/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4108,43 +4111,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I349" tableType="xml" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87" connectionId="1">
-  <autoFilter ref="A19:I349" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Both"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I349" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I349" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A52:I64">
     <sortCondition descending="1" ref="F19:F349"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="86">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="85">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="84">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="83">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="82">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="81">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="80">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="79">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="78">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4153,12 +4150,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4488,9 +4485,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -4543,127 +4538,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="75.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="30.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="45" t="s">
         <v>432</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -4676,12 +4671,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
@@ -4694,12 +4689,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -4712,12 +4707,12 @@
       <c r="C14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -4730,60 +4725,60 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="61.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="47" t="s">
         <v>563</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -5521,7 +5516,7 @@
     </row>
     <row r="48" spans="1:9" ht="30">
       <c r="A48" s="21" t="s">
-        <v>205</v>
+        <v>777</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>255</v>
@@ -6912,7 +6907,7 @@
       </c>
       <c r="I102" s="31"/>
     </row>
-    <row r="103" spans="1:9" ht="45" hidden="1">
+    <row r="103" spans="1:9" ht="45">
       <c r="A103" s="29" t="s">
         <v>97</v>
       </c>
@@ -6937,7 +6932,7 @@
       </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="45" hidden="1">
+    <row r="104" spans="1:9" ht="45">
       <c r="A104" s="29" t="s">
         <v>98</v>
       </c>
@@ -7364,7 +7359,7 @@
       </c>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="1:9" hidden="1">
+    <row r="121" spans="1:9">
       <c r="A121" s="29" t="s">
         <v>115</v>
       </c>
@@ -7389,7 +7384,7 @@
       </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:9" ht="30" hidden="1">
+    <row r="122" spans="1:9" ht="30">
       <c r="A122" s="29" t="s">
         <v>116</v>
       </c>
@@ -7414,7 +7409,7 @@
       </c>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="1:9" ht="30" hidden="1">
+    <row r="123" spans="1:9" ht="30">
       <c r="A123" s="29" t="s">
         <v>117</v>
       </c>
@@ -7439,7 +7434,7 @@
       </c>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="1:9" ht="30" hidden="1">
+    <row r="124" spans="1:9" ht="30">
       <c r="A124" s="29" t="s">
         <v>118</v>
       </c>
@@ -7464,7 +7459,7 @@
       </c>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="1:9" ht="30" hidden="1">
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="29" t="s">
         <v>119</v>
       </c>
@@ -8905,7 +8900,7 @@
       </c>
       <c r="I181" s="34"/>
     </row>
-    <row r="182" spans="1:9" ht="45" hidden="1">
+    <row r="182" spans="1:9" ht="45">
       <c r="A182" s="29" t="s">
         <v>138</v>
       </c>
@@ -8930,7 +8925,7 @@
       </c>
       <c r="I182" s="31"/>
     </row>
-    <row r="183" spans="1:9" ht="30" hidden="1">
+    <row r="183" spans="1:9" ht="30">
       <c r="A183" s="29" t="s">
         <v>139</v>
       </c>
@@ -8955,7 +8950,7 @@
       </c>
       <c r="I183" s="31"/>
     </row>
-    <row r="184" spans="1:9" ht="30" hidden="1">
+    <row r="184" spans="1:9" ht="30">
       <c r="A184" s="21" t="s">
         <v>140</v>
       </c>
@@ -8980,7 +8975,7 @@
       </c>
       <c r="I184" s="31"/>
     </row>
-    <row r="185" spans="1:9" ht="30" hidden="1">
+    <row r="185" spans="1:9" ht="30">
       <c r="A185" s="21" t="s">
         <v>683</v>
       </c>
@@ -9005,7 +9000,7 @@
       </c>
       <c r="I185" s="34"/>
     </row>
-    <row r="186" spans="1:9" ht="45" hidden="1">
+    <row r="186" spans="1:9" ht="45">
       <c r="A186" s="29" t="s">
         <v>141</v>
       </c>
@@ -9030,7 +9025,7 @@
       </c>
       <c r="I186" s="31"/>
     </row>
-    <row r="187" spans="1:9" ht="240" hidden="1">
+    <row r="187" spans="1:9" ht="240">
       <c r="A187" s="29" t="s">
         <v>142</v>
       </c>
@@ -9055,7 +9050,7 @@
       </c>
       <c r="I187" s="31"/>
     </row>
-    <row r="188" spans="1:9" ht="45" hidden="1">
+    <row r="188" spans="1:9" ht="45">
       <c r="A188" s="29" t="s">
         <v>143</v>
       </c>
@@ -9532,7 +9527,7 @@
       </c>
       <c r="I206" s="31"/>
     </row>
-    <row r="207" spans="1:9" hidden="1">
+    <row r="207" spans="1:9">
       <c r="A207" s="29" t="s">
         <v>156</v>
       </c>
@@ -9557,7 +9552,7 @@
       </c>
       <c r="I207" s="31"/>
     </row>
-    <row r="208" spans="1:9" ht="30" hidden="1">
+    <row r="208" spans="1:9" ht="30">
       <c r="A208" s="29" t="s">
         <v>157</v>
       </c>
@@ -10682,7 +10677,7 @@
       </c>
       <c r="I252" s="31"/>
     </row>
-    <row r="253" spans="1:9" ht="30" hidden="1">
+    <row r="253" spans="1:9" ht="30">
       <c r="A253" s="29" t="s">
         <v>182</v>
       </c>
@@ -10707,7 +10702,7 @@
       </c>
       <c r="I253" s="31"/>
     </row>
-    <row r="254" spans="1:9" hidden="1">
+    <row r="254" spans="1:9">
       <c r="A254" s="29" t="s">
         <v>183</v>
       </c>
@@ -10732,7 +10727,7 @@
       </c>
       <c r="I254" s="31"/>
     </row>
-    <row r="255" spans="1:9" ht="45" hidden="1">
+    <row r="255" spans="1:9" ht="45">
       <c r="A255" s="29" t="s">
         <v>184</v>
       </c>
@@ -10757,7 +10752,7 @@
       </c>
       <c r="I255" s="31"/>
     </row>
-    <row r="256" spans="1:9" hidden="1">
+    <row r="256" spans="1:9">
       <c r="A256" s="29" t="s">
         <v>185</v>
       </c>
@@ -10782,7 +10777,7 @@
       </c>
       <c r="I256" s="31"/>
     </row>
-    <row r="257" spans="1:9" ht="45" hidden="1">
+    <row r="257" spans="1:9" ht="45">
       <c r="A257" s="29" t="s">
         <v>186</v>
       </c>
@@ -10807,7 +10802,7 @@
       </c>
       <c r="I257" s="31"/>
     </row>
-    <row r="258" spans="1:9" ht="45" hidden="1">
+    <row r="258" spans="1:9" ht="45">
       <c r="A258" s="29" t="s">
         <v>187</v>
       </c>
@@ -10832,7 +10827,7 @@
       </c>
       <c r="I258" s="31"/>
     </row>
-    <row r="259" spans="1:9" ht="30" hidden="1">
+    <row r="259" spans="1:9" ht="30">
       <c r="A259" s="29" t="s">
         <v>188</v>
       </c>
@@ -10907,7 +10902,7 @@
       </c>
       <c r="I261" s="31"/>
     </row>
-    <row r="262" spans="1:9" ht="30" hidden="1">
+    <row r="262" spans="1:9" ht="30">
       <c r="A262" s="29" t="s">
         <v>191</v>
       </c>
@@ -11690,7 +11685,7 @@
       </c>
       <c r="I292" s="31"/>
     </row>
-    <row r="293" spans="1:9" ht="30" hidden="1">
+    <row r="293" spans="1:9" ht="30">
       <c r="A293" s="29" t="s">
         <v>204</v>
       </c>
@@ -11715,7 +11710,7 @@
       </c>
       <c r="I293" s="31"/>
     </row>
-    <row r="294" spans="1:9" ht="30" hidden="1">
+    <row r="294" spans="1:9" ht="30">
       <c r="A294" s="29" t="s">
         <v>205</v>
       </c>
@@ -13207,6 +13202,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -13214,272 +13214,267 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A345:I346 A226:H226 B198:I198 A199:I225 A20:I197 A227:I339">
-    <cfRule type="expression" dxfId="69" priority="139">
+    <cfRule type="expression" dxfId="88" priority="139">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="140">
+    <cfRule type="expression" dxfId="87" priority="140">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="147">
+    <cfRule type="expression" dxfId="86" priority="147">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A345:I346 A226:H226 B198:I198 A199:I225 A20:I197 A227:I339">
-    <cfRule type="expression" dxfId="66" priority="93">
+    <cfRule type="expression" dxfId="85" priority="93">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="94">
+    <cfRule type="expression" dxfId="84" priority="94">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="95">
+    <cfRule type="expression" dxfId="83" priority="95">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F345:F346 F20:F339">
-    <cfRule type="expression" dxfId="63" priority="99">
+    <cfRule type="expression" dxfId="82" priority="99">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="100">
+    <cfRule type="expression" dxfId="81" priority="100">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343:I343">
-    <cfRule type="expression" dxfId="61" priority="44">
+    <cfRule type="expression" dxfId="80" priority="44">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="45">
+    <cfRule type="expression" dxfId="79" priority="45">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="46">
+    <cfRule type="expression" dxfId="78" priority="46">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A343:I343">
-    <cfRule type="expression" dxfId="58" priority="39">
+    <cfRule type="expression" dxfId="77" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="40">
+    <cfRule type="expression" dxfId="76" priority="40">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="41">
+    <cfRule type="expression" dxfId="75" priority="41">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F343">
-    <cfRule type="expression" dxfId="55" priority="42">
+    <cfRule type="expression" dxfId="74" priority="42">
       <formula>NOT(VLOOKUP(F343,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="43">
+    <cfRule type="expression" dxfId="73" priority="43">
       <formula>(VLOOKUP(F343,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A348:I348">
-    <cfRule type="expression" dxfId="53" priority="76">
+    <cfRule type="expression" dxfId="72" priority="76">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="77">
+    <cfRule type="expression" dxfId="71" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="78">
+    <cfRule type="expression" dxfId="70" priority="78">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A348:I348">
-    <cfRule type="expression" dxfId="50" priority="71">
+    <cfRule type="expression" dxfId="69" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="72">
+    <cfRule type="expression" dxfId="68" priority="72">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="73">
+    <cfRule type="expression" dxfId="67" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F348">
-    <cfRule type="expression" dxfId="47" priority="74">
+    <cfRule type="expression" dxfId="66" priority="74">
       <formula>NOT(VLOOKUP(F348,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="75">
+    <cfRule type="expression" dxfId="65" priority="75">
       <formula>(VLOOKUP(F348,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A340:I340">
-    <cfRule type="expression" dxfId="45" priority="60">
+    <cfRule type="expression" dxfId="64" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="61">
+    <cfRule type="expression" dxfId="63" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="62">
+    <cfRule type="expression" dxfId="62" priority="62">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A340:I340">
-    <cfRule type="expression" dxfId="42" priority="55">
+    <cfRule type="expression" dxfId="61" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="56">
+    <cfRule type="expression" dxfId="60" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="57">
+    <cfRule type="expression" dxfId="59" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F340">
-    <cfRule type="expression" dxfId="39" priority="58">
+    <cfRule type="expression" dxfId="58" priority="58">
       <formula>NOT(VLOOKUP(F340,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="59">
+    <cfRule type="expression" dxfId="57" priority="59">
       <formula>(VLOOKUP(F340,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A341:I342">
-    <cfRule type="expression" dxfId="37" priority="52">
+    <cfRule type="expression" dxfId="56" priority="52">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="53">
+    <cfRule type="expression" dxfId="55" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="54">
+    <cfRule type="expression" dxfId="54" priority="54">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A341:I342">
-    <cfRule type="expression" dxfId="34" priority="47">
+    <cfRule type="expression" dxfId="53" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="48">
+    <cfRule type="expression" dxfId="52" priority="48">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="49">
+    <cfRule type="expression" dxfId="51" priority="49">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F341:F342">
-    <cfRule type="expression" dxfId="31" priority="50">
+    <cfRule type="expression" dxfId="50" priority="50">
       <formula>NOT(VLOOKUP(F341,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="51">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>(VLOOKUP(F341,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A344:I344">
-    <cfRule type="expression" dxfId="29" priority="36">
+    <cfRule type="expression" dxfId="48" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="37">
+    <cfRule type="expression" dxfId="47" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="38">
+    <cfRule type="expression" dxfId="46" priority="38">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A344:I344">
-    <cfRule type="expression" dxfId="26" priority="31">
+    <cfRule type="expression" dxfId="45" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="32">
+    <cfRule type="expression" dxfId="44" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="33">
+    <cfRule type="expression" dxfId="43" priority="33">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F344">
-    <cfRule type="expression" dxfId="23" priority="34">
+    <cfRule type="expression" dxfId="42" priority="34">
       <formula>NOT(VLOOKUP(F344,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35">
+    <cfRule type="expression" dxfId="41" priority="35">
       <formula>(VLOOKUP(F344,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347:I347">
-    <cfRule type="expression" dxfId="21" priority="20">
+    <cfRule type="expression" dxfId="40" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="39" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347:I347">
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F347">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>NOT(VLOOKUP(F347,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="33" priority="19">
       <formula>(VLOOKUP(F347,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A349:H349">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A349:H349">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="29" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="27" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F349">
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>NOT(VLOOKUP(F349,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="11">
+    <cfRule type="expression" dxfId="25" priority="11">
       <formula>(VLOOKUP(F349,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I349">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I349">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update RS of MS-OXWSMSG and add  MS-OXWSTASK SHOLDMAY config
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSMSG/MS-OXWSMSG_RequirementSpecification.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EABAA239-24BB-46BA-8BFD-ED43F6928875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18946DFB-332D-4E0E-A58B-AF2963E04660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$349</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$337</definedName>
     <definedName name="Appendix_A_Target_14" localSheetId="0">Requirements!$A$198</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="756">
   <si>
     <t>Req ID</t>
   </si>
@@ -2021,12 +2021,6 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does introduce the VotingInformation element. (This element was introduced in Exchange 2013 SP1.)</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R182001</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R182002</t>
   </si>
   <si>
     <t>MS-OXWSMSG_R182003</t>
@@ -2658,9 +2652,6 @@
     <t>[In t:SendPromptType Simple Type]The value "VotingOption" means the user is prompted to confirm their choice before sending a response.</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the ApprovalRequestDataType complex type. (&lt;1&gt; Section 2.2.4: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the ApprovalRequestDataType complex type. )</t>
-  </si>
-  <si>
     <t>[In Appendix C: Product Behavior] Implementation does introduce the ApprovalRequestDataType complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
   </si>
   <si>
@@ -2670,30 +2661,6 @@
     <t>[In Appendix C: Product Behavior] Implementation does not support the VotingInformation element. (&lt;9&gt; Section 2.2.4.3:  Exchange 2007,Exchange 2010, and the initial release of Exchange 2013 do not support the VotingInformation element. )</t>
   </si>
   <si>
-    <t>MS-OXWSMSG_R352</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R353</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R354</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R355</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R356</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R357</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R358</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R359</t>
-  </si>
-  <si>
     <t>MS-OXWSMSG_R360</t>
   </si>
   <si>
@@ -2709,33 +2676,6 @@
     <t>[In Appendix C: Product Behavior] Implementation does introduce the ArrayOfVotingOptionDataType complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the ReminderMessageDataType complex type. (&lt;3&gt; Section 2.2.4: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the ReminderMessageDataType complex type. )</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does introduce the ReminderMessageDataType complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the VotingInformationType complex type. (&lt;4&gt; Section 2.2.4: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the VotingInformationType complex type. )</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does introduce the VotingInformationType complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the ArrayOfVotingOptionDataType complex type. (&lt;2&gt; Section 2.2.4: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the ArrayOfVotingOptionDataType complex type. )</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the VotingOptionDataType complex type. (&lt;5&gt; Section 2.2.4: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the VotingOptionDataType complex type. )</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does introduce the VotingOptionDataType complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the ovalRequestDataTypAppre complex type. (&lt;6&gt; Section 2.2.4.1: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the ovalRequestDataTypAppre complex type. )</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does introduce the ovalRequestDataTypAppre complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
-  </si>
-  <si>
     <t>[In Appendix C: Product Behavior] Implementation does not support the ArrayOfVotingOptionDataType complex type. (&lt;7&gt; Section 2.2.4.2: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the ArrayOfVotingOptionDataType  complex type. )</t>
   </si>
   <si>
@@ -2769,9 +2709,6 @@
     <t>MS-OXWSMSG_R371</t>
   </si>
   <si>
-    <t>MS-OXWSMSG_R372</t>
-  </si>
-  <si>
     <t>[In Appendix C: Product Behavior] Implementation does not support the ReminderMessageDataType complex type. (&lt;11&gt; Section 2.2.4.4:  Exchange 2007,Exchange 2010, and the initial release of Exchange 2013 do not support the ReminderMessageDataType complex type. )</t>
   </si>
   <si>
@@ -2788,12 +2725,6 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does introduce the VotingOptionDataType complex type. (This type was introduced in Exchange 2013 SP1.)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the SendPromptType simple type. (&lt;14&gt; Section 2.2.5:  Exchange 2007,Exchange 2010, and the initial release of Exchange 2013 do not support the SendPromptType simple type. )</t>
-  </si>
-  <si>
-    <t>MS-OXWSMSG_R373</t>
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does introduce the SendPromptType complex type. (This type was introduced in Exchange 2013 SP1.)</t>
@@ -2913,6 +2844,9 @@
   </si>
   <si>
     <t>MS-OXWSMSG_R444</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the ApprovalRequestDataType complex type. (&lt;6&gt; Section 2.2.4.1: Exchange 2007, Exchange 2010, and the initial release of Exchange 2013 do not support the ovalRequestDataTypAppre complex type. )</t>
   </si>
 </sst>
 </file>
@@ -3217,6 +3151,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3240,21 +3189,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4111,10 +4045,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I349" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I349" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I337" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I337" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A52:I64">
-    <sortCondition descending="1" ref="F19:F349"/>
+    <sortCondition descending="1" ref="F19:F337"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
@@ -4483,7 +4417,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L350"/>
+  <dimension ref="A1:L338"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4538,127 +4472,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="75.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="30.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="50" t="s">
         <v>432</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -4671,12 +4605,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
@@ -4689,12 +4623,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -4707,12 +4641,12 @@
       <c r="C14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -4725,60 +4659,60 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="61.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
-        <v>563</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="B17" s="52" t="s">
+        <v>561</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -5466,13 +5400,13 @@
     </row>
     <row r="46" spans="1:9" ht="30">
       <c r="A46" s="21" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B46" s="23" t="s">
         <v>255</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32" t="s">
@@ -5491,13 +5425,13 @@
     </row>
     <row r="47" spans="1:9" ht="30">
       <c r="A47" s="21" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>255</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D47" s="32"/>
       <c r="E47" s="32" t="s">
@@ -5516,13 +5450,13 @@
     </row>
     <row r="48" spans="1:9" ht="30">
       <c r="A48" s="21" t="s">
-        <v>777</v>
+        <v>754</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>255</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -5541,13 +5475,13 @@
     </row>
     <row r="49" spans="1:9" ht="30">
       <c r="A49" s="21" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B49" s="33" t="s">
         <v>255</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D49" s="32"/>
       <c r="E49" s="32" t="s">
@@ -5566,13 +5500,13 @@
     </row>
     <row r="50" spans="1:9" ht="30">
       <c r="A50" s="21" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B50" s="33" t="s">
         <v>255</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D50" s="32"/>
       <c r="E50" s="32" t="s">
@@ -5591,13 +5525,13 @@
     </row>
     <row r="51" spans="1:9" ht="30">
       <c r="A51" s="21" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B51" s="33" t="s">
         <v>255</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D51" s="32"/>
       <c r="E51" s="32" t="s">
@@ -5616,13 +5550,13 @@
     </row>
     <row r="52" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A52" s="32" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D52" s="32"/>
       <c r="E52" s="32" t="s">
@@ -5638,18 +5572,18 @@
         <v>17</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>757</v>
+        <v>734</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="37" customFormat="1" ht="195.75" customHeight="1">
       <c r="A53" s="21" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B53" s="33" t="s">
+        <v>576</v>
+      </c>
+      <c r="C53" s="19" t="s">
         <v>578</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>580</v>
       </c>
       <c r="D53" s="32"/>
       <c r="E53" s="32" t="s">
@@ -5668,13 +5602,13 @@
     </row>
     <row r="54" spans="1:9" s="37" customFormat="1" ht="78" customHeight="1">
       <c r="A54" s="21" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B54" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D54" s="32"/>
       <c r="E54" s="32" t="s">
@@ -5693,13 +5627,13 @@
     </row>
     <row r="55" spans="1:9" s="37" customFormat="1" ht="34.5" customHeight="1">
       <c r="A55" s="21" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D55" s="32"/>
       <c r="E55" s="32" t="s">
@@ -5718,13 +5652,13 @@
     </row>
     <row r="56" spans="1:9" s="37" customFormat="1" ht="48" customHeight="1">
       <c r="A56" s="21" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D56" s="32"/>
       <c r="E56" s="32" t="s">
@@ -5743,16 +5677,16 @@
     </row>
     <row r="57" spans="1:9" s="37" customFormat="1" ht="51" customHeight="1">
       <c r="A57" s="21" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E57" s="32" t="s">
         <v>19</v>
@@ -5770,16 +5704,16 @@
     </row>
     <row r="58" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A58" s="21" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E58" s="32" t="s">
         <v>19</v>
@@ -5797,13 +5731,13 @@
     </row>
     <row r="59" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A59" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="B59" s="33" t="s">
         <v>576</v>
       </c>
-      <c r="B59" s="33" t="s">
-        <v>578</v>
-      </c>
       <c r="C59" s="19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D59" s="32"/>
       <c r="E59" s="32" t="s">
@@ -5822,13 +5756,13 @@
     </row>
     <row r="60" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A60" s="21" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D60" s="32"/>
       <c r="E60" s="32" t="s">
@@ -5847,13 +5781,13 @@
     </row>
     <row r="61" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A61" s="21" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D61" s="32"/>
       <c r="E61" s="32" t="s">
@@ -5872,13 +5806,13 @@
     </row>
     <row r="62" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A62" s="21" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B62" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D62" s="32"/>
       <c r="E62" s="32" t="s">
@@ -5897,13 +5831,13 @@
     </row>
     <row r="63" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A63" s="21" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D63" s="32"/>
       <c r="E63" s="32" t="s">
@@ -5922,13 +5856,13 @@
     </row>
     <row r="64" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A64" s="21" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D64" s="32"/>
       <c r="E64" s="32" t="s">
@@ -5947,13 +5881,13 @@
     </row>
     <row r="65" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A65" s="21" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D65" s="32"/>
       <c r="E65" s="32" t="s">
@@ -5969,18 +5903,18 @@
         <v>17</v>
       </c>
       <c r="I65" s="19" t="s">
-        <v>759</v>
+        <v>736</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="37" customFormat="1" ht="120">
       <c r="A66" s="21" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B66" s="33" t="s">
+        <v>611</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>613</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>615</v>
       </c>
       <c r="D66" s="32"/>
       <c r="E66" s="32" t="s">
@@ -5999,13 +5933,13 @@
     </row>
     <row r="67" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A67" s="21" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D67" s="32"/>
       <c r="E67" s="32" t="s">
@@ -6024,13 +5958,13 @@
     </row>
     <row r="68" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A68" s="21" t="s">
+        <v>609</v>
+      </c>
+      <c r="B68" s="33" t="s">
         <v>611</v>
       </c>
-      <c r="B68" s="33" t="s">
-        <v>613</v>
-      </c>
       <c r="C68" s="19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D68" s="32"/>
       <c r="E68" s="32" t="s">
@@ -6049,13 +5983,13 @@
     </row>
     <row r="69" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A69" s="21" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D69" s="32"/>
       <c r="E69" s="32" t="s">
@@ -6077,7 +6011,7 @@
         <v>64</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C70" s="19" t="s">
         <v>444</v>
@@ -6102,7 +6036,7 @@
         <v>65</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C71" s="19" t="s">
         <v>445</v>
@@ -6127,7 +6061,7 @@
         <v>66</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C72" s="19" t="s">
         <v>446</v>
@@ -6152,7 +6086,7 @@
         <v>67</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C73" s="19" t="s">
         <v>289</v>
@@ -6177,7 +6111,7 @@
         <v>68</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C74" s="19" t="s">
         <v>447</v>
@@ -6202,7 +6136,7 @@
         <v>69</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C75" s="19" t="s">
         <v>290</v>
@@ -6229,7 +6163,7 @@
         <v>70</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C76" s="31" t="s">
         <v>291</v>
@@ -6256,7 +6190,7 @@
         <v>71</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C77" s="31" t="s">
         <v>292</v>
@@ -6281,7 +6215,7 @@
         <v>72</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C78" s="31" t="s">
         <v>293</v>
@@ -6306,7 +6240,7 @@
         <v>73</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C79" s="31" t="s">
         <v>294</v>
@@ -6331,7 +6265,7 @@
         <v>74</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C80" s="19" t="s">
         <v>448</v>
@@ -6356,7 +6290,7 @@
         <v>75</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C81" s="31" t="s">
         <v>295</v>
@@ -6383,7 +6317,7 @@
         <v>76</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C82" s="19" t="s">
         <v>296</v>
@@ -6410,7 +6344,7 @@
         <v>77</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C83" s="19" t="s">
         <v>449</v>
@@ -6435,7 +6369,7 @@
         <v>78</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C84" s="31" t="s">
         <v>297</v>
@@ -6460,7 +6394,7 @@
         <v>79</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C85" s="31" t="s">
         <v>298</v>
@@ -6485,7 +6419,7 @@
         <v>80</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C86" s="31" t="s">
         <v>299</v>
@@ -6510,7 +6444,7 @@
         <v>81</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C87" s="19" t="s">
         <v>451</v>
@@ -6535,7 +6469,7 @@
         <v>82</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C88" s="31" t="s">
         <v>300</v>
@@ -6560,7 +6494,7 @@
         <v>83</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C89" s="31" t="s">
         <v>301</v>
@@ -6585,7 +6519,7 @@
         <v>84</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C90" s="31" t="s">
         <v>302</v>
@@ -6610,7 +6544,7 @@
         <v>85</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C91" s="19" t="s">
         <v>450</v>
@@ -6635,7 +6569,7 @@
         <v>86</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C92" s="31" t="s">
         <v>303</v>
@@ -6660,7 +6594,7 @@
         <v>87</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C93" s="31" t="s">
         <v>304</v>
@@ -6685,10 +6619,10 @@
         <v>88</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29" t="s">
@@ -6710,7 +6644,7 @@
         <v>89</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C95" s="31" t="s">
         <v>305</v>
@@ -6735,7 +6669,7 @@
         <v>90</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C96" s="31" t="s">
         <v>306</v>
@@ -6760,7 +6694,7 @@
         <v>91</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C97" s="31" t="s">
         <v>307</v>
@@ -6785,7 +6719,7 @@
         <v>92</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C98" s="31" t="s">
         <v>308</v>
@@ -6810,7 +6744,7 @@
         <v>93</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C99" s="31" t="s">
         <v>309</v>
@@ -6837,7 +6771,7 @@
         <v>94</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C100" s="31" t="s">
         <v>310</v>
@@ -6862,7 +6796,7 @@
         <v>95</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C101" s="31" t="s">
         <v>311</v>
@@ -6887,7 +6821,7 @@
         <v>96</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C102" s="31" t="s">
         <v>312</v>
@@ -6912,7 +6846,7 @@
         <v>97</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C103" s="31" t="s">
         <v>313</v>
@@ -6937,7 +6871,7 @@
         <v>98</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C104" s="31" t="s">
         <v>314</v>
@@ -6964,7 +6898,7 @@
         <v>99</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C105" s="19" t="s">
         <v>452</v>
@@ -6989,7 +6923,7 @@
         <v>100</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C106" s="19" t="s">
         <v>453</v>
@@ -7014,7 +6948,7 @@
         <v>101</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C107" s="31" t="s">
         <v>315</v>
@@ -7039,7 +6973,7 @@
         <v>102</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C108" s="19" t="s">
         <v>454</v>
@@ -7064,10 +6998,10 @@
         <v>103</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29" t="s">
@@ -7089,7 +7023,7 @@
         <v>104</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C110" s="31" t="s">
         <v>316</v>
@@ -7114,7 +7048,7 @@
         <v>105</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C111" s="31" t="s">
         <v>317</v>
@@ -7139,10 +7073,10 @@
         <v>106</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29" t="s">
@@ -7164,7 +7098,7 @@
         <v>107</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C113" s="31" t="s">
         <v>318</v>
@@ -7189,7 +7123,7 @@
         <v>108</v>
       </c>
       <c r="B114" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C114" s="31" t="s">
         <v>319</v>
@@ -7214,7 +7148,7 @@
         <v>109</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C115" s="31" t="s">
         <v>320</v>
@@ -7239,7 +7173,7 @@
         <v>110</v>
       </c>
       <c r="B116" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C116" s="31" t="s">
         <v>321</v>
@@ -7264,7 +7198,7 @@
         <v>111</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C117" s="31" t="s">
         <v>322</v>
@@ -7289,7 +7223,7 @@
         <v>112</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C118" s="31" t="s">
         <v>323</v>
@@ -7314,7 +7248,7 @@
         <v>113</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C119" s="31" t="s">
         <v>324</v>
@@ -7339,7 +7273,7 @@
         <v>114</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C120" s="19" t="s">
         <v>455</v>
@@ -7364,7 +7298,7 @@
         <v>115</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C121" s="31" t="s">
         <v>325</v>
@@ -7389,7 +7323,7 @@
         <v>116</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C122" s="31" t="s">
         <v>326</v>
@@ -7414,7 +7348,7 @@
         <v>117</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C123" s="19" t="s">
         <v>456</v>
@@ -7439,7 +7373,7 @@
         <v>118</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C124" s="31" t="s">
         <v>327</v>
@@ -7464,7 +7398,7 @@
         <v>119</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C125" s="31" t="s">
         <v>328</v>
@@ -7491,7 +7425,7 @@
         <v>120</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C126" s="31" t="s">
         <v>329</v>
@@ -7516,7 +7450,7 @@
         <v>121</v>
       </c>
       <c r="B127" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C127" s="19" t="s">
         <v>457</v>
@@ -7541,7 +7475,7 @@
         <v>122</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C128" s="31" t="s">
         <v>330</v>
@@ -7566,7 +7500,7 @@
         <v>123</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C129" s="31" t="s">
         <v>331</v>
@@ -7591,7 +7525,7 @@
         <v>124</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C130" s="31" t="s">
         <v>332</v>
@@ -7616,7 +7550,7 @@
         <v>125</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C131" s="31" t="s">
         <v>333</v>
@@ -7643,7 +7577,7 @@
         <v>126</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C132" s="31" t="s">
         <v>334</v>
@@ -7668,7 +7602,7 @@
         <v>127</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C133" s="31" t="s">
         <v>335</v>
@@ -7693,7 +7627,7 @@
         <v>128</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C134" s="31" t="s">
         <v>336</v>
@@ -7718,7 +7652,7 @@
         <v>129</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C135" s="31" t="s">
         <v>337</v>
@@ -7743,7 +7677,7 @@
         <v>130</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C136" s="31" t="s">
         <v>338</v>
@@ -7768,7 +7702,7 @@
         <v>131</v>
       </c>
       <c r="B137" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C137" s="19" t="s">
         <v>458</v>
@@ -7793,7 +7727,7 @@
         <v>132</v>
       </c>
       <c r="B138" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C138" s="31" t="s">
         <v>339</v>
@@ -7818,7 +7752,7 @@
         <v>133</v>
       </c>
       <c r="B139" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C139" s="31" t="s">
         <v>340</v>
@@ -7843,10 +7777,10 @@
         <v>134</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="29" t="s">
@@ -7868,7 +7802,7 @@
         <v>135</v>
       </c>
       <c r="B141" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C141" s="19" t="s">
         <v>341</v>
@@ -7893,7 +7827,7 @@
         <v>460</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C142" s="34" t="s">
         <v>459</v>
@@ -7918,7 +7852,7 @@
         <v>136</v>
       </c>
       <c r="B143" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C143" s="31" t="s">
         <v>342</v>
@@ -7943,7 +7877,7 @@
         <v>137</v>
       </c>
       <c r="B144" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C144" s="19" t="s">
         <v>343</v>
@@ -7968,7 +7902,7 @@
         <v>462</v>
       </c>
       <c r="B145" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C145" s="19" t="s">
         <v>461</v>
@@ -7993,10 +7927,10 @@
         <v>463</v>
       </c>
       <c r="B146" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D146" s="32"/>
       <c r="E146" s="32" t="s">
@@ -8018,10 +7952,10 @@
         <v>464</v>
       </c>
       <c r="B147" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C147" s="19" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D147" s="32"/>
       <c r="E147" s="32" t="s">
@@ -8037,18 +7971,18 @@
         <v>17</v>
       </c>
       <c r="I147" s="19" t="s">
-        <v>769</v>
+        <v>746</v>
       </c>
     </row>
     <row r="148" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A148" s="21" t="s">
-        <v>771</v>
+        <v>748</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C148" s="19" t="s">
-        <v>772</v>
+        <v>749</v>
       </c>
       <c r="D148" s="32"/>
       <c r="E148" s="32" t="s">
@@ -8070,10 +8004,10 @@
         <v>465</v>
       </c>
       <c r="B149" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C149" s="19" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D149" s="32"/>
       <c r="E149" s="32" t="s">
@@ -8095,10 +8029,10 @@
         <v>466</v>
       </c>
       <c r="B150" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C150" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D150" s="32"/>
       <c r="E150" s="32" t="s">
@@ -8114,18 +8048,18 @@
         <v>17</v>
       </c>
       <c r="I150" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="151" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A151" s="21" t="s">
-        <v>775</v>
+        <v>752</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C151" s="19" t="s">
-        <v>773</v>
+        <v>750</v>
       </c>
       <c r="D151" s="32"/>
       <c r="E151" s="32" t="s">
@@ -8147,10 +8081,10 @@
         <v>467</v>
       </c>
       <c r="B152" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C152" s="19" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D152" s="32"/>
       <c r="E152" s="32" t="s">
@@ -8172,10 +8106,10 @@
         <v>468</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C153" s="19" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D153" s="32"/>
       <c r="E153" s="32" t="s">
@@ -8191,18 +8125,18 @@
         <v>17</v>
       </c>
       <c r="I153" s="19" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="154" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A154" s="21" t="s">
-        <v>776</v>
+        <v>753</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C154" s="19" t="s">
-        <v>774</v>
+        <v>751</v>
       </c>
       <c r="D154" s="32"/>
       <c r="E154" s="32" t="s">
@@ -8221,13 +8155,13 @@
     </row>
     <row r="155" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A155" s="21" t="s">
+        <v>623</v>
+      </c>
+      <c r="B155" s="23" t="s">
         <v>625</v>
       </c>
-      <c r="B155" s="23" t="s">
-        <v>627</v>
-      </c>
       <c r="C155" s="19" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D155" s="32"/>
       <c r="E155" s="32" t="s">
@@ -8243,18 +8177,18 @@
         <v>17</v>
       </c>
       <c r="I155" s="19" t="s">
-        <v>762</v>
+        <v>739</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="37" customFormat="1" ht="180">
       <c r="A156" s="21" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B156" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C156" s="19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D156" s="32"/>
       <c r="E156" s="32" t="s">
@@ -8273,13 +8207,13 @@
     </row>
     <row r="157" spans="1:9" s="37" customFormat="1" ht="60">
       <c r="A157" s="21" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B157" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C157" s="19" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D157" s="32"/>
       <c r="E157" s="32" t="s">
@@ -8298,13 +8232,13 @@
     </row>
     <row r="158" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A158" s="21" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B158" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C158" s="19" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D158" s="32"/>
       <c r="E158" s="32" t="s">
@@ -8323,13 +8257,13 @@
     </row>
     <row r="159" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A159" s="21" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B159" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C159" s="19" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D159" s="32"/>
       <c r="E159" s="32" t="s">
@@ -8348,13 +8282,13 @@
     </row>
     <row r="160" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A160" s="21" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B160" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C160" s="19" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D160" s="32"/>
       <c r="E160" s="32" t="s">
@@ -8373,13 +8307,13 @@
     </row>
     <row r="161" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A161" s="21" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D161" s="32"/>
       <c r="E161" s="32" t="s">
@@ -8398,13 +8332,13 @@
     </row>
     <row r="162" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A162" s="21" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B162" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C162" s="19" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D162" s="32"/>
       <c r="E162" s="32" t="s">
@@ -8423,13 +8357,13 @@
     </row>
     <row r="163" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A163" s="21" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B163" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C163" s="19" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D163" s="32"/>
       <c r="E163" s="32" t="s">
@@ -8448,13 +8382,13 @@
     </row>
     <row r="164" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A164" s="21" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B164" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C164" s="19" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D164" s="32"/>
       <c r="E164" s="32" t="s">
@@ -8473,13 +8407,13 @@
     </row>
     <row r="165" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A165" s="21" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B165" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C165" s="19" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D165" s="32"/>
       <c r="E165" s="32" t="s">
@@ -8498,13 +8432,13 @@
     </row>
     <row r="166" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A166" s="21" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B166" s="33" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C166" s="19" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D166" s="32"/>
       <c r="E166" s="32" t="s">
@@ -8523,13 +8457,13 @@
     </row>
     <row r="167" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A167" s="21" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C167" s="19" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D167" s="32"/>
       <c r="E167" s="32" t="s">
@@ -8548,13 +8482,13 @@
     </row>
     <row r="168" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A168" s="21" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C168" s="19" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D168" s="32"/>
       <c r="E168" s="32" t="s">
@@ -8570,18 +8504,18 @@
         <v>17</v>
       </c>
       <c r="I168" s="19" t="s">
-        <v>764</v>
+        <v>741</v>
       </c>
     </row>
     <row r="169" spans="1:9" s="37" customFormat="1" ht="120">
       <c r="A169" s="21" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B169" s="33" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C169" s="19" t="s">
-        <v>770</v>
+        <v>747</v>
       </c>
       <c r="D169" s="32"/>
       <c r="E169" s="32" t="s">
@@ -8600,13 +8534,13 @@
     </row>
     <row r="170" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A170" s="21" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B170" s="33" t="s">
+        <v>659</v>
+      </c>
+      <c r="C170" s="19" t="s">
         <v>661</v>
-      </c>
-      <c r="C170" s="19" t="s">
-        <v>663</v>
       </c>
       <c r="D170" s="32"/>
       <c r="E170" s="32" t="s">
@@ -8625,13 +8559,13 @@
     </row>
     <row r="171" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A171" s="21" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B171" s="33" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C171" s="19" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D171" s="32"/>
       <c r="E171" s="32" t="s">
@@ -8650,13 +8584,13 @@
     </row>
     <row r="172" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A172" s="21" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B172" s="33" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C172" s="19" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D172" s="32"/>
       <c r="E172" s="32" t="s">
@@ -8675,13 +8609,13 @@
     </row>
     <row r="173" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A173" s="21" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B173" s="33" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C173" s="19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D173" s="32"/>
       <c r="E173" s="32" t="s">
@@ -8700,13 +8634,13 @@
     </row>
     <row r="174" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A174" s="21" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B174" s="33" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C174" s="19" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D174" s="32"/>
       <c r="E174" s="32" t="s">
@@ -8725,13 +8659,13 @@
     </row>
     <row r="175" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A175" s="21" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B175" s="23" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C175" s="19" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D175" s="32"/>
       <c r="E175" s="32" t="s">
@@ -8747,18 +8681,18 @@
         <v>17</v>
       </c>
       <c r="I175" s="19" t="s">
-        <v>766</v>
+        <v>743</v>
       </c>
     </row>
     <row r="176" spans="1:9" s="37" customFormat="1" ht="120">
       <c r="A176" s="21" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B176" s="23" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C176" s="19" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D176" s="32"/>
       <c r="E176" s="32" t="s">
@@ -8777,13 +8711,13 @@
     </row>
     <row r="177" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A177" s="21" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B177" s="33" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C177" s="19" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D177" s="32"/>
       <c r="E177" s="32" t="s">
@@ -8802,13 +8736,13 @@
     </row>
     <row r="178" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A178" s="21" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B178" s="33" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C178" s="19" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D178" s="32"/>
       <c r="E178" s="32" t="s">
@@ -8827,13 +8761,13 @@
     </row>
     <row r="179" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A179" s="21" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B179" s="33" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C179" s="19" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D179" s="32"/>
       <c r="E179" s="32" t="s">
@@ -8852,13 +8786,13 @@
     </row>
     <row r="180" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A180" s="21" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B180" s="33" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C180" s="19" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D180" s="32"/>
       <c r="E180" s="32" t="s">
@@ -8877,13 +8811,13 @@
     </row>
     <row r="181" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A181" s="21" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B181" s="33" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C181" s="19" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D181" s="32"/>
       <c r="E181" s="32" t="s">
@@ -8908,7 +8842,7 @@
         <v>256</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -8958,7 +8892,7 @@
         <v>256</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -8977,13 +8911,13 @@
     </row>
     <row r="185" spans="1:9" ht="30">
       <c r="A185" s="21" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B185" s="23" t="s">
         <v>256</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D185" s="32"/>
       <c r="E185" s="32" t="s">
@@ -9302,13 +9236,13 @@
     </row>
     <row r="198" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A198" s="38" t="s">
+        <v>683</v>
+      </c>
+      <c r="B198" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="C198" s="19" t="s">
         <v>685</v>
-      </c>
-      <c r="B198" s="23" t="s">
-        <v>686</v>
-      </c>
-      <c r="C198" s="19" t="s">
-        <v>687</v>
       </c>
       <c r="D198" s="32"/>
       <c r="E198" s="32" t="s">
@@ -9324,18 +9258,18 @@
         <v>17</v>
       </c>
       <c r="I198" s="19" t="s">
-        <v>768</v>
+        <v>745</v>
       </c>
     </row>
     <row r="199" spans="1:9" s="37" customFormat="1" ht="120">
       <c r="A199" s="21" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B199" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="C199" s="19" t="s">
         <v>686</v>
-      </c>
-      <c r="C199" s="19" t="s">
-        <v>688</v>
       </c>
       <c r="D199" s="32"/>
       <c r="E199" s="32" t="s">
@@ -9354,13 +9288,13 @@
     </row>
     <row r="200" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A200" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="B200" s="23" t="s">
+        <v>684</v>
+      </c>
+      <c r="C200" s="19" t="s">
         <v>690</v>
-      </c>
-      <c r="B200" s="23" t="s">
-        <v>686</v>
-      </c>
-      <c r="C200" s="19" t="s">
-        <v>692</v>
       </c>
       <c r="D200" s="32"/>
       <c r="E200" s="32" t="s">
@@ -9379,13 +9313,13 @@
     </row>
     <row r="201" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A201" s="21" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B201" s="23" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C201" s="19" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D201" s="32"/>
       <c r="E201" s="32" t="s">
@@ -9404,13 +9338,13 @@
     </row>
     <row r="202" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A202" s="21" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B202" s="23" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C202" s="19" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D202" s="21"/>
       <c r="E202" s="21" t="s">
@@ -9429,13 +9363,13 @@
     </row>
     <row r="203" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A203" s="21" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B203" s="23" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C203" s="19" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D203" s="21"/>
       <c r="E203" s="21" t="s">
@@ -10951,7 +10885,7 @@
         <v>17</v>
       </c>
       <c r="I263" s="19" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="30">
@@ -10978,7 +10912,7 @@
         <v>17</v>
       </c>
       <c r="I264" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="265" spans="1:9" ht="60">
@@ -11005,7 +10939,7 @@
         <v>17</v>
       </c>
       <c r="I265" s="19" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="266" spans="1:9" ht="30">
@@ -11032,7 +10966,7 @@
         <v>17</v>
       </c>
       <c r="I266" s="19" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="267" spans="1:9" ht="45">
@@ -11585,7 +11519,7 @@
       </c>
       <c r="I288" s="31"/>
     </row>
-    <row r="289" spans="1:9" ht="30">
+    <row r="289" spans="1:10" ht="30">
       <c r="A289" s="29" t="s">
         <v>200</v>
       </c>
@@ -11610,7 +11544,7 @@
       </c>
       <c r="I289" s="31"/>
     </row>
-    <row r="290" spans="1:9" ht="75">
+    <row r="290" spans="1:10" ht="75">
       <c r="A290" s="29" t="s">
         <v>201</v>
       </c>
@@ -11635,7 +11569,7 @@
       </c>
       <c r="I290" s="31"/>
     </row>
-    <row r="291" spans="1:9" ht="330">
+    <row r="291" spans="1:10" ht="330">
       <c r="A291" s="29" t="s">
         <v>202</v>
       </c>
@@ -11660,7 +11594,7 @@
       </c>
       <c r="I291" s="31"/>
     </row>
-    <row r="292" spans="1:9" ht="30">
+    <row r="292" spans="1:10" ht="30">
       <c r="A292" s="29" t="s">
         <v>203</v>
       </c>
@@ -11685,7 +11619,7 @@
       </c>
       <c r="I292" s="31"/>
     </row>
-    <row r="293" spans="1:9" ht="30">
+    <row r="293" spans="1:10" ht="30">
       <c r="A293" s="29" t="s">
         <v>204</v>
       </c>
@@ -11710,7 +11644,7 @@
       </c>
       <c r="I293" s="31"/>
     </row>
-    <row r="294" spans="1:9" ht="30">
+    <row r="294" spans="1:10" ht="30">
       <c r="A294" s="29" t="s">
         <v>205</v>
       </c>
@@ -11735,7 +11669,7 @@
       </c>
       <c r="I294" s="31"/>
     </row>
-    <row r="295" spans="1:9" ht="45">
+    <row r="295" spans="1:10" ht="45">
       <c r="A295" s="29" t="s">
         <v>206</v>
       </c>
@@ -11760,7 +11694,7 @@
       </c>
       <c r="I295" s="31"/>
     </row>
-    <row r="296" spans="1:9" ht="75">
+    <row r="296" spans="1:10" ht="75">
       <c r="A296" s="29" t="s">
         <v>207</v>
       </c>
@@ -11785,7 +11719,7 @@
       </c>
       <c r="I296" s="31"/>
     </row>
-    <row r="297" spans="1:9" ht="60">
+    <row r="297" spans="1:10" ht="60">
       <c r="A297" s="29" t="s">
         <v>208</v>
       </c>
@@ -11810,7 +11744,7 @@
       </c>
       <c r="I297" s="31"/>
     </row>
-    <row r="298" spans="1:9" ht="45">
+    <row r="298" spans="1:10" ht="45">
       <c r="A298" s="21" t="s">
         <v>524</v>
       </c>
@@ -11835,7 +11769,7 @@
       </c>
       <c r="I298" s="34"/>
     </row>
-    <row r="299" spans="1:9" ht="60">
+    <row r="299" spans="1:10" ht="60">
       <c r="A299" s="21" t="s">
         <v>525</v>
       </c>
@@ -11860,7 +11794,7 @@
       </c>
       <c r="I299" s="34"/>
     </row>
-    <row r="300" spans="1:9" ht="30">
+    <row r="300" spans="1:10" ht="30">
       <c r="A300" s="29" t="s">
         <v>209</v>
       </c>
@@ -11885,7 +11819,7 @@
       </c>
       <c r="I300" s="31"/>
     </row>
-    <row r="301" spans="1:9" s="37" customFormat="1" ht="60">
+    <row r="301" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A301" s="29" t="s">
         <v>238</v>
       </c>
@@ -11910,7 +11844,7 @@
       </c>
       <c r="I301" s="31"/>
     </row>
-    <row r="302" spans="1:9" s="37" customFormat="1" ht="45">
+    <row r="302" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A302" s="29" t="s">
         <v>239</v>
       </c>
@@ -11939,7 +11873,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="303" spans="1:9" s="37" customFormat="1" ht="30">
+    <row r="303" spans="1:10" s="37" customFormat="1" ht="30">
       <c r="A303" s="29" t="s">
         <v>240</v>
       </c>
@@ -11964,21 +11898,23 @@
       </c>
       <c r="I303" s="31"/>
     </row>
-    <row r="304" spans="1:9" s="37" customFormat="1" ht="60">
+    <row r="304" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A304" s="21" t="s">
-        <v>528</v>
-      </c>
-      <c r="B304" s="30" t="s">
-        <v>270</v>
+        <v>699</v>
+      </c>
+      <c r="B304" s="36">
+        <v>8</v>
       </c>
       <c r="C304" s="19" t="s">
-        <v>698</v>
-      </c>
-      <c r="D304" s="32"/>
-      <c r="E304" s="29" t="s">
+        <v>755</v>
+      </c>
+      <c r="D304" s="21" t="s">
+        <v>735</v>
+      </c>
+      <c r="E304" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F304" s="29" t="s">
+      <c r="F304" s="32" t="s">
         <v>3</v>
       </c>
       <c r="G304" s="32" t="s">
@@ -11988,22 +11924,25 @@
         <v>18</v>
       </c>
       <c r="I304" s="19"/>
+      <c r="J304" s="39"/>
     </row>
     <row r="305" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A305" s="21" t="s">
-        <v>529</v>
-      </c>
-      <c r="B305" s="35">
+        <v>700</v>
+      </c>
+      <c r="B305" s="36">
         <v>8</v>
       </c>
       <c r="C305" s="19" t="s">
-        <v>699</v>
-      </c>
-      <c r="D305" s="32"/>
-      <c r="E305" s="29" t="s">
+        <v>696</v>
+      </c>
+      <c r="D305" s="21" t="s">
+        <v>735</v>
+      </c>
+      <c r="E305" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F305" s="29" t="s">
+      <c r="F305" s="32" t="s">
         <v>3</v>
       </c>
       <c r="G305" s="32" t="s">
@@ -12017,15 +11956,17 @@
     </row>
     <row r="306" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A306" s="21" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B306" s="36">
         <v>8</v>
       </c>
       <c r="C306" s="19" t="s">
-        <v>719</v>
-      </c>
-      <c r="D306" s="32"/>
+        <v>704</v>
+      </c>
+      <c r="D306" s="21" t="s">
+        <v>737</v>
+      </c>
       <c r="E306" s="32" t="s">
         <v>22</v>
       </c>
@@ -12043,15 +11984,17 @@
     </row>
     <row r="307" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A307" s="21" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B307" s="36">
         <v>8</v>
       </c>
       <c r="C307" s="19" t="s">
-        <v>714</v>
-      </c>
-      <c r="D307" s="32"/>
+        <v>703</v>
+      </c>
+      <c r="D307" s="21" t="s">
+        <v>737</v>
+      </c>
       <c r="E307" s="32" t="s">
         <v>22</v>
       </c>
@@ -12069,15 +12012,17 @@
     </row>
     <row r="308" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A308" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="B308" s="36">
+        <v>705</v>
+      </c>
+      <c r="B308" s="35">
         <v>8</v>
       </c>
       <c r="C308" s="19" t="s">
-        <v>715</v>
-      </c>
-      <c r="D308" s="32"/>
+        <v>707</v>
+      </c>
+      <c r="D308" s="21" t="s">
+        <v>532</v>
+      </c>
       <c r="E308" s="32" t="s">
         <v>22</v>
       </c>
@@ -12095,15 +12040,17 @@
     </row>
     <row r="309" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A309" s="21" t="s">
-        <v>705</v>
-      </c>
-      <c r="B309" s="36">
+        <v>706</v>
+      </c>
+      <c r="B309" s="35">
         <v>8</v>
       </c>
       <c r="C309" s="19" t="s">
-        <v>716</v>
-      </c>
-      <c r="D309" s="32"/>
+        <v>708</v>
+      </c>
+      <c r="D309" s="21" t="s">
+        <v>532</v>
+      </c>
       <c r="E309" s="32" t="s">
         <v>22</v>
       </c>
@@ -12121,19 +12068,21 @@
     </row>
     <row r="310" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A310" s="21" t="s">
-        <v>706</v>
-      </c>
-      <c r="B310" s="36">
-        <v>8</v>
+        <v>528</v>
+      </c>
+      <c r="B310" s="30" t="s">
+        <v>270</v>
       </c>
       <c r="C310" s="19" t="s">
-        <v>717</v>
-      </c>
-      <c r="D310" s="32"/>
-      <c r="E310" s="32" t="s">
+        <v>698</v>
+      </c>
+      <c r="D310" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="E310" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F310" s="32" t="s">
+      <c r="F310" s="29" t="s">
         <v>3</v>
       </c>
       <c r="G310" s="32" t="s">
@@ -12147,19 +12096,21 @@
     </row>
     <row r="311" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A311" s="21" t="s">
-        <v>707</v>
-      </c>
-      <c r="B311" s="36">
-        <v>8</v>
+        <v>529</v>
+      </c>
+      <c r="B311" s="30" t="s">
+        <v>270</v>
       </c>
       <c r="C311" s="19" t="s">
-        <v>718</v>
-      </c>
-      <c r="D311" s="32"/>
-      <c r="E311" s="32" t="s">
+        <v>527</v>
+      </c>
+      <c r="D311" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="E311" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F311" s="32" t="s">
+      <c r="F311" s="29" t="s">
         <v>3</v>
       </c>
       <c r="G311" s="32" t="s">
@@ -12173,19 +12124,21 @@
     </row>
     <row r="312" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A312" s="21" t="s">
-        <v>708</v>
-      </c>
-      <c r="B312" s="36">
-        <v>8</v>
+        <v>530</v>
+      </c>
+      <c r="B312" s="30" t="s">
+        <v>270</v>
       </c>
       <c r="C312" s="19" t="s">
-        <v>720</v>
-      </c>
-      <c r="D312" s="32"/>
-      <c r="E312" s="32" t="s">
+        <v>697</v>
+      </c>
+      <c r="D312" s="32" t="s">
+        <v>534</v>
+      </c>
+      <c r="E312" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F312" s="32" t="s">
+      <c r="F312" s="29" t="s">
         <v>3</v>
       </c>
       <c r="G312" s="32" t="s">
@@ -12199,19 +12152,21 @@
     </row>
     <row r="313" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A313" s="21" t="s">
-        <v>709</v>
-      </c>
-      <c r="B313" s="36">
-        <v>8</v>
+        <v>531</v>
+      </c>
+      <c r="B313" s="30" t="s">
+        <v>270</v>
       </c>
       <c r="C313" s="19" t="s">
-        <v>721</v>
-      </c>
-      <c r="D313" s="32"/>
-      <c r="E313" s="32" t="s">
+        <v>526</v>
+      </c>
+      <c r="D313" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="E313" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F313" s="32" t="s">
+      <c r="F313" s="29" t="s">
         <v>3</v>
       </c>
       <c r="G313" s="32" t="s">
@@ -12225,16 +12180,16 @@
     </row>
     <row r="314" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A314" s="21" t="s">
-        <v>710</v>
-      </c>
-      <c r="B314" s="36">
+        <v>709</v>
+      </c>
+      <c r="B314" s="35">
         <v>8</v>
       </c>
       <c r="C314" s="19" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
       <c r="D314" s="21" t="s">
-        <v>758</v>
+        <v>738</v>
       </c>
       <c r="E314" s="32" t="s">
         <v>22</v>
@@ -12253,16 +12208,16 @@
     </row>
     <row r="315" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A315" s="21" t="s">
-        <v>711</v>
-      </c>
-      <c r="B315" s="36">
+        <v>710</v>
+      </c>
+      <c r="B315" s="35">
         <v>8</v>
       </c>
       <c r="C315" s="19" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="D315" s="21" t="s">
-        <v>758</v>
+        <v>738</v>
       </c>
       <c r="E315" s="32" t="s">
         <v>22</v>
@@ -12281,16 +12236,16 @@
     </row>
     <row r="316" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A316" s="21" t="s">
-        <v>712</v>
-      </c>
-      <c r="B316" s="36">
+        <v>711</v>
+      </c>
+      <c r="B316" s="35">
         <v>8</v>
       </c>
       <c r="C316" s="19" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
       <c r="D316" s="21" t="s">
-        <v>760</v>
+        <v>740</v>
       </c>
       <c r="E316" s="32" t="s">
         <v>22</v>
@@ -12309,16 +12264,16 @@
     </row>
     <row r="317" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A317" s="21" t="s">
-        <v>713</v>
-      </c>
-      <c r="B317" s="36">
+        <v>712</v>
+      </c>
+      <c r="B317" s="35">
         <v>8</v>
       </c>
       <c r="C317" s="19" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="D317" s="21" t="s">
-        <v>760</v>
+        <v>740</v>
       </c>
       <c r="E317" s="32" t="s">
         <v>22</v>
@@ -12332,21 +12287,21 @@
       <c r="H317" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I317" s="19"/>
+      <c r="I317" s="34"/>
       <c r="J317" s="39"/>
     </row>
     <row r="318" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A318" s="21" t="s">
-        <v>725</v>
+        <v>713</v>
       </c>
       <c r="B318" s="35">
         <v>8</v>
       </c>
       <c r="C318" s="19" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="D318" s="21" t="s">
-        <v>534</v>
+        <v>742</v>
       </c>
       <c r="E318" s="32" t="s">
         <v>22</v>
@@ -12360,21 +12315,21 @@
       <c r="H318" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I318" s="19"/>
+      <c r="I318" s="34"/>
       <c r="J318" s="39"/>
     </row>
     <row r="319" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A319" s="21" t="s">
-        <v>726</v>
+        <v>714</v>
       </c>
       <c r="B319" s="35">
         <v>8</v>
       </c>
       <c r="C319" s="19" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="D319" s="21" t="s">
-        <v>534</v>
+        <v>742</v>
       </c>
       <c r="E319" s="32" t="s">
         <v>22</v>
@@ -12388,26 +12343,26 @@
       <c r="H319" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I319" s="19"/>
+      <c r="I319" s="34"/>
       <c r="J319" s="39"/>
     </row>
     <row r="320" spans="1:10" s="37" customFormat="1" ht="60">
       <c r="A320" s="21" t="s">
-        <v>530</v>
-      </c>
-      <c r="B320" s="30" t="s">
-        <v>270</v>
+        <v>722</v>
+      </c>
+      <c r="B320" s="35">
+        <v>8</v>
       </c>
       <c r="C320" s="19" t="s">
-        <v>701</v>
-      </c>
-      <c r="D320" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="E320" s="29" t="s">
+        <v>724</v>
+      </c>
+      <c r="D320" s="21" t="s">
+        <v>744</v>
+      </c>
+      <c r="E320" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F320" s="29" t="s">
+      <c r="F320" s="32" t="s">
         <v>3</v>
       </c>
       <c r="G320" s="32" t="s">
@@ -12416,26 +12371,26 @@
       <c r="H320" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I320" s="19"/>
+      <c r="I320" s="34"/>
       <c r="J320" s="39"/>
     </row>
     <row r="321" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A321" s="21" t="s">
-        <v>531</v>
-      </c>
-      <c r="B321" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="C321" s="19" t="s">
-        <v>527</v>
-      </c>
-      <c r="D321" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="E321" s="29" t="s">
+        <v>723</v>
+      </c>
+      <c r="B321" s="35">
+        <v>8</v>
+      </c>
+      <c r="C321" s="34" t="s">
+        <v>721</v>
+      </c>
+      <c r="D321" s="21" t="s">
+        <v>744</v>
+      </c>
+      <c r="E321" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F321" s="29" t="s">
+      <c r="F321" s="32" t="s">
         <v>3</v>
       </c>
       <c r="G321" s="32" t="s">
@@ -12444,404 +12399,384 @@
       <c r="H321" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I321" s="19"/>
+      <c r="I321" s="34"/>
       <c r="J321" s="39"/>
     </row>
-    <row r="322" spans="1:10" s="37" customFormat="1" ht="60">
+    <row r="322" spans="1:10" s="37" customFormat="1" ht="210">
       <c r="A322" s="21" t="s">
-        <v>532</v>
-      </c>
-      <c r="B322" s="30" t="s">
-        <v>270</v>
+        <v>241</v>
+      </c>
+      <c r="B322" s="23" t="s">
+        <v>725</v>
       </c>
       <c r="C322" s="19" t="s">
-        <v>700</v>
-      </c>
-      <c r="D322" s="32" t="s">
-        <v>536</v>
-      </c>
+        <v>726</v>
+      </c>
+      <c r="D322" s="29"/>
       <c r="E322" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F322" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G322" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H322" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I322" s="19"/>
+      <c r="G322" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H322" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I322" s="31"/>
       <c r="J322" s="39"/>
     </row>
-    <row r="323" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A323" s="21" t="s">
-        <v>533</v>
-      </c>
-      <c r="B323" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="C323" s="19" t="s">
-        <v>526</v>
-      </c>
-      <c r="D323" s="21" t="s">
-        <v>536</v>
-      </c>
+    <row r="323" spans="1:10" s="37" customFormat="1" ht="47.25" customHeight="1">
+      <c r="A323" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="B323" s="23" t="s">
+        <v>725</v>
+      </c>
+      <c r="C323" s="31" t="s">
+        <v>411</v>
+      </c>
+      <c r="D323" s="29"/>
       <c r="E323" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F323" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G323" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H323" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I323" s="19"/>
+      <c r="G323" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H323" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I323" s="19" t="s">
+        <v>564</v>
+      </c>
       <c r="J323" s="39"/>
     </row>
     <row r="324" spans="1:10" s="37" customFormat="1" ht="60">
-      <c r="A324" s="21" t="s">
+      <c r="A324" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="B324" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="C324" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="D324" s="29"/>
+      <c r="E324" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F324" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G324" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H324" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I324" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="J324" s="39"/>
+    </row>
+    <row r="325" spans="1:10" s="37" customFormat="1" ht="105">
+      <c r="A325" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="B325" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="C325" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="D325" s="29"/>
+      <c r="E325" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F325" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G325" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H325" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I325" s="31"/>
+    </row>
+    <row r="326" spans="1:10" s="37" customFormat="1" ht="180">
+      <c r="A326" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B326" s="23" t="s">
+        <v>728</v>
+      </c>
+      <c r="C326" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="D326" s="29"/>
+      <c r="E326" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F326" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G326" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H326" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I326" s="31"/>
+      <c r="J326" s="39"/>
+    </row>
+    <row r="327" spans="1:10" s="37" customFormat="1" ht="409.5">
+      <c r="A327" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B327" s="23" t="s">
         <v>729</v>
       </c>
-      <c r="B324" s="35">
-        <v>8</v>
-      </c>
-      <c r="C324" s="19" t="s">
-        <v>736</v>
-      </c>
-      <c r="D324" s="21" t="s">
-        <v>761</v>
-      </c>
-      <c r="E324" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F324" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G324" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H324" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I324" s="19"/>
-      <c r="J324" s="39"/>
-    </row>
-    <row r="325" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A325" s="21" t="s">
+      <c r="C327" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D327" s="29"/>
+      <c r="E327" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F327" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G327" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H327" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I327" s="31"/>
+    </row>
+    <row r="328" spans="1:10" s="37" customFormat="1" ht="45">
+      <c r="A328" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="B328" s="23" t="s">
+        <v>731</v>
+      </c>
+      <c r="C328" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="B325" s="35">
-        <v>8</v>
-      </c>
-      <c r="C325" s="19" t="s">
-        <v>737</v>
-      </c>
-      <c r="D325" s="21" t="s">
-        <v>761</v>
-      </c>
-      <c r="E325" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F325" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G325" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H325" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I325" s="19"/>
-      <c r="J325" s="39"/>
-    </row>
-    <row r="326" spans="1:10" s="37" customFormat="1" ht="60">
-      <c r="A326" s="21" t="s">
+      <c r="D328" s="21"/>
+      <c r="E328" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F328" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G328" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H328" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I328" s="19"/>
+    </row>
+    <row r="329" spans="1:10" s="37" customFormat="1" ht="30">
+      <c r="A329" s="21" t="s">
+        <v>558</v>
+      </c>
+      <c r="B329" s="23" t="s">
         <v>731</v>
       </c>
-      <c r="B326" s="35">
-        <v>8</v>
-      </c>
-      <c r="C326" s="19" t="s">
-        <v>738</v>
-      </c>
-      <c r="D326" s="21" t="s">
-        <v>763</v>
-      </c>
-      <c r="E326" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F326" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G326" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H326" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I326" s="19"/>
-      <c r="J326" s="39"/>
-    </row>
-    <row r="327" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A327" s="21" t="s">
-        <v>732</v>
-      </c>
-      <c r="B327" s="35">
-        <v>8</v>
-      </c>
-      <c r="C327" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="D327" s="21" t="s">
-        <v>763</v>
-      </c>
-      <c r="E327" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F327" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G327" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H327" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I327" s="34"/>
-      <c r="J327" s="39"/>
-    </row>
-    <row r="328" spans="1:10" s="37" customFormat="1" ht="60">
-      <c r="A328" s="21" t="s">
-        <v>733</v>
-      </c>
-      <c r="B328" s="35">
-        <v>8</v>
-      </c>
-      <c r="C328" s="19" t="s">
-        <v>740</v>
-      </c>
-      <c r="D328" s="21" t="s">
-        <v>765</v>
-      </c>
-      <c r="E328" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F328" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G328" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H328" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I328" s="34"/>
-      <c r="J328" s="39"/>
-    </row>
-    <row r="329" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A329" s="21" t="s">
-        <v>734</v>
-      </c>
-      <c r="B329" s="35">
-        <v>8</v>
-      </c>
       <c r="C329" s="19" t="s">
-        <v>741</v>
+        <v>538</v>
       </c>
       <c r="D329" s="21" t="s">
-        <v>765</v>
-      </c>
-      <c r="E329" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F329" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G329" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H329" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I329" s="34"/>
-      <c r="J329" s="39"/>
-    </row>
-    <row r="330" spans="1:10" s="37" customFormat="1" ht="60">
+        <v>539</v>
+      </c>
+      <c r="E329" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F329" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G329" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H329" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I329" s="19"/>
+    </row>
+    <row r="330" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A330" s="21" t="s">
-        <v>735</v>
-      </c>
-      <c r="B330" s="35">
-        <v>8</v>
+        <v>559</v>
+      </c>
+      <c r="B330" s="23" t="s">
+        <v>731</v>
       </c>
       <c r="C330" s="19" t="s">
-        <v>742</v>
-      </c>
-      <c r="D330" s="32"/>
-      <c r="E330" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F330" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G330" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H330" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I330" s="34"/>
-      <c r="J330" s="39"/>
+        <v>540</v>
+      </c>
+      <c r="D330" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="E330" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F330" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G330" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H330" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I330" s="19"/>
     </row>
     <row r="331" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A331" s="21" t="s">
-        <v>743</v>
-      </c>
-      <c r="B331" s="35">
-        <v>8</v>
+        <v>542</v>
+      </c>
+      <c r="B331" s="23" t="s">
+        <v>731</v>
       </c>
       <c r="C331" s="19" t="s">
-        <v>744</v>
-      </c>
-      <c r="D331" s="32"/>
-      <c r="E331" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F331" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G331" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H331" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I331" s="34"/>
-      <c r="J331" s="39"/>
-    </row>
-    <row r="332" spans="1:10" s="37" customFormat="1" ht="60">
+        <v>543</v>
+      </c>
+      <c r="D331" s="21"/>
+      <c r="E331" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F331" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G331" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H331" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I331" s="19"/>
+    </row>
+    <row r="332" spans="1:10" s="37" customFormat="1" ht="45">
       <c r="A332" s="21" t="s">
-        <v>745</v>
-      </c>
-      <c r="B332" s="35">
-        <v>8</v>
+        <v>545</v>
+      </c>
+      <c r="B332" s="23" t="s">
+        <v>731</v>
       </c>
       <c r="C332" s="19" t="s">
-        <v>747</v>
-      </c>
-      <c r="D332" s="21" t="s">
-        <v>767</v>
-      </c>
-      <c r="E332" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F332" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G332" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H332" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I332" s="34"/>
-      <c r="J332" s="39"/>
-    </row>
-    <row r="333" spans="1:10" s="37" customFormat="1" ht="45">
+        <v>546</v>
+      </c>
+      <c r="D332" s="21"/>
+      <c r="E332" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F332" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G332" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H332" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I332" s="19"/>
+    </row>
+    <row r="333" spans="1:10" s="37" customFormat="1" ht="30">
       <c r="A333" s="21" t="s">
-        <v>746</v>
-      </c>
-      <c r="B333" s="35">
-        <v>8</v>
-      </c>
-      <c r="C333" s="34" t="s">
-        <v>744</v>
+        <v>552</v>
+      </c>
+      <c r="B333" s="23" t="s">
+        <v>731</v>
+      </c>
+      <c r="C333" s="19" t="s">
+        <v>553</v>
       </c>
       <c r="D333" s="21" t="s">
-        <v>767</v>
-      </c>
-      <c r="E333" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F333" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G333" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H333" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I333" s="34"/>
-      <c r="J333" s="39"/>
-    </row>
-    <row r="334" spans="1:10" s="37" customFormat="1" ht="210">
+        <v>554</v>
+      </c>
+      <c r="E333" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F333" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G333" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H333" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I333" s="19"/>
+    </row>
+    <row r="334" spans="1:10" s="37" customFormat="1" ht="30">
       <c r="A334" s="21" t="s">
-        <v>241</v>
+        <v>555</v>
       </c>
       <c r="B334" s="23" t="s">
-        <v>748</v>
+        <v>731</v>
       </c>
       <c r="C334" s="19" t="s">
-        <v>749</v>
-      </c>
-      <c r="D334" s="29"/>
-      <c r="E334" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F334" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G334" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H334" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I334" s="31"/>
-      <c r="J334" s="39"/>
-    </row>
-    <row r="335" spans="1:10" s="37" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A335" s="29" t="s">
-        <v>242</v>
+        <v>556</v>
+      </c>
+      <c r="D334" s="21" t="s">
+        <v>554</v>
+      </c>
+      <c r="E334" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F334" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G334" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H334" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I334" s="19"/>
+    </row>
+    <row r="335" spans="1:10" s="37" customFormat="1" ht="45">
+      <c r="A335" s="21" t="s">
+        <v>550</v>
       </c>
       <c r="B335" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="C335" s="31" t="s">
-        <v>411</v>
-      </c>
-      <c r="D335" s="29"/>
-      <c r="E335" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F335" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G335" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H335" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I335" s="19" t="s">
-        <v>566</v>
-      </c>
-      <c r="J335" s="39"/>
-    </row>
-    <row r="336" spans="1:10" s="37" customFormat="1" ht="60">
-      <c r="A336" s="29" t="s">
-        <v>243</v>
+        <v>731</v>
+      </c>
+      <c r="C335" s="19" t="s">
+        <v>551</v>
+      </c>
+      <c r="D335" s="21"/>
+      <c r="E335" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F335" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G335" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H335" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I335" s="19"/>
+    </row>
+    <row r="336" spans="1:10" s="37" customFormat="1" ht="135">
+      <c r="A336" s="21" t="s">
+        <v>247</v>
       </c>
       <c r="B336" s="23" t="s">
-        <v>750</v>
+        <v>732</v>
       </c>
       <c r="C336" s="19" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D336" s="29"/>
       <c r="E336" s="29" t="s">
@@ -12854,359 +12789,42 @@
         <v>15</v>
       </c>
       <c r="H336" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I336" s="19" t="s">
-        <v>428</v>
-      </c>
-      <c r="J336" s="39"/>
-    </row>
-    <row r="337" spans="1:10" s="37" customFormat="1" ht="105">
-      <c r="A337" s="29" t="s">
-        <v>244</v>
+        <v>21</v>
+      </c>
+      <c r="I336" s="31"/>
+    </row>
+    <row r="337" spans="1:9" s="37" customFormat="1" ht="45">
+      <c r="A337" s="21" t="s">
+        <v>565</v>
       </c>
       <c r="B337" s="23" t="s">
-        <v>750</v>
+        <v>560</v>
       </c>
       <c r="C337" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="D337" s="29"/>
-      <c r="E337" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F337" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G337" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H337" s="29" t="s">
+        <v>733</v>
+      </c>
+      <c r="D337" s="21"/>
+      <c r="E337" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F337" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G337" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H337" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I337" s="31"/>
-    </row>
-    <row r="338" spans="1:10" s="37" customFormat="1" ht="180">
-      <c r="A338" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="B338" s="23" t="s">
-        <v>751</v>
-      </c>
-      <c r="C338" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="D338" s="29"/>
-      <c r="E338" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F338" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G338" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H338" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I338" s="31"/>
-      <c r="J338" s="39"/>
-    </row>
-    <row r="339" spans="1:10" s="37" customFormat="1" ht="409.5">
-      <c r="A339" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="B339" s="23" t="s">
-        <v>752</v>
-      </c>
-      <c r="C339" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="D339" s="29"/>
-      <c r="E339" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F339" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G339" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H339" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I339" s="31"/>
-    </row>
-    <row r="340" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A340" s="21" t="s">
-        <v>539</v>
-      </c>
-      <c r="B340" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C340" s="19" t="s">
-        <v>753</v>
-      </c>
-      <c r="D340" s="21"/>
-      <c r="E340" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F340" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G340" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H340" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I340" s="19"/>
-    </row>
-    <row r="341" spans="1:10" s="37" customFormat="1" ht="30">
-      <c r="A341" s="21" t="s">
-        <v>560</v>
-      </c>
-      <c r="B341" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C341" s="19" t="s">
-        <v>540</v>
-      </c>
-      <c r="D341" s="21" t="s">
-        <v>541</v>
-      </c>
-      <c r="E341" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F341" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G341" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H341" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I341" s="19"/>
-    </row>
-    <row r="342" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A342" s="21" t="s">
-        <v>561</v>
-      </c>
-      <c r="B342" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C342" s="19" t="s">
-        <v>542</v>
-      </c>
-      <c r="D342" s="21" t="s">
-        <v>541</v>
-      </c>
-      <c r="E342" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F342" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G342" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H342" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I342" s="19"/>
-    </row>
-    <row r="343" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A343" s="21" t="s">
-        <v>544</v>
-      </c>
-      <c r="B343" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C343" s="19" t="s">
-        <v>545</v>
-      </c>
-      <c r="D343" s="21"/>
-      <c r="E343" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F343" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G343" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H343" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I343" s="19"/>
-    </row>
-    <row r="344" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A344" s="21" t="s">
-        <v>547</v>
-      </c>
-      <c r="B344" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C344" s="19" t="s">
-        <v>548</v>
-      </c>
-      <c r="D344" s="21"/>
-      <c r="E344" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F344" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G344" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H344" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I344" s="19"/>
-    </row>
-    <row r="345" spans="1:10" s="37" customFormat="1" ht="30">
-      <c r="A345" s="21" t="s">
-        <v>554</v>
-      </c>
-      <c r="B345" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C345" s="19" t="s">
-        <v>555</v>
-      </c>
-      <c r="D345" s="21" t="s">
-        <v>556</v>
-      </c>
-      <c r="E345" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F345" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G345" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H345" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I345" s="19"/>
-    </row>
-    <row r="346" spans="1:10" s="37" customFormat="1" ht="30">
-      <c r="A346" s="21" t="s">
-        <v>557</v>
-      </c>
-      <c r="B346" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C346" s="19" t="s">
-        <v>558</v>
-      </c>
-      <c r="D346" s="21" t="s">
-        <v>556</v>
-      </c>
-      <c r="E346" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F346" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G346" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H346" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I346" s="19"/>
-    </row>
-    <row r="347" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A347" s="21" t="s">
-        <v>552</v>
-      </c>
-      <c r="B347" s="23" t="s">
-        <v>754</v>
-      </c>
-      <c r="C347" s="19" t="s">
-        <v>553</v>
-      </c>
-      <c r="D347" s="21"/>
-      <c r="E347" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F347" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G347" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H347" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I347" s="19"/>
-    </row>
-    <row r="348" spans="1:10" s="37" customFormat="1" ht="135">
-      <c r="A348" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="B348" s="23" t="s">
-        <v>755</v>
-      </c>
-      <c r="C348" s="19" t="s">
-        <v>416</v>
-      </c>
-      <c r="D348" s="29"/>
-      <c r="E348" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F348" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G348" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H348" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I348" s="31"/>
-    </row>
-    <row r="349" spans="1:10" s="37" customFormat="1" ht="45">
-      <c r="A349" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="B349" s="23" t="s">
-        <v>562</v>
-      </c>
-      <c r="C349" s="19" t="s">
-        <v>756</v>
-      </c>
-      <c r="D349" s="21"/>
-      <c r="E349" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F349" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G349" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H349" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I349" s="31" t="s">
+      <c r="I337" s="31" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="350" spans="1:10" s="37" customFormat="1">
-      <c r="B350" s="40"/>
+    <row r="338" spans="1:9" s="37" customFormat="1">
+      <c r="B338" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -13214,9 +12832,14 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A345:I346 A226:H226 B198:I198 A199:I225 A20:I197 A227:I339">
+  <conditionalFormatting sqref="A333:I334 A226:H226 B198:I198 A199:I225 A20:I197 A227:I327">
     <cfRule type="expression" dxfId="88" priority="139">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13227,7 +12850,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A345:I346 A226:H226 B198:I198 A199:I225 A20:I197 A227:I339">
+  <conditionalFormatting sqref="A333:I334 A226:H226 B198:I198 A199:I225 A20:I197 A227:I327">
     <cfRule type="expression" dxfId="85" priority="93">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13238,7 +12861,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F345:F346 F20:F339">
+  <conditionalFormatting sqref="F333:F334 F20:F327">
     <cfRule type="expression" dxfId="82" priority="99">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -13246,7 +12869,7 @@
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A343:I343">
+  <conditionalFormatting sqref="A331:I331">
     <cfRule type="expression" dxfId="80" priority="44">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13257,7 +12880,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A343:I343">
+  <conditionalFormatting sqref="A331:I331">
     <cfRule type="expression" dxfId="77" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13268,15 +12891,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F343">
+  <conditionalFormatting sqref="F331">
     <cfRule type="expression" dxfId="74" priority="42">
-      <formula>NOT(VLOOKUP(F343,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F331,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="73" priority="43">
-      <formula>(VLOOKUP(F343,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F331,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A348:I348">
+  <conditionalFormatting sqref="A336:I336">
     <cfRule type="expression" dxfId="72" priority="76">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13287,7 +12910,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A348:I348">
+  <conditionalFormatting sqref="A336:I336">
     <cfRule type="expression" dxfId="69" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13298,15 +12921,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F348">
+  <conditionalFormatting sqref="F336">
     <cfRule type="expression" dxfId="66" priority="74">
-      <formula>NOT(VLOOKUP(F348,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F336,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="65" priority="75">
-      <formula>(VLOOKUP(F348,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F336,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A340:I340">
+  <conditionalFormatting sqref="A328:I328">
     <cfRule type="expression" dxfId="64" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13317,7 +12940,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A340:I340">
+  <conditionalFormatting sqref="A328:I328">
     <cfRule type="expression" dxfId="61" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13328,15 +12951,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F340">
+  <conditionalFormatting sqref="F328">
     <cfRule type="expression" dxfId="58" priority="58">
-      <formula>NOT(VLOOKUP(F340,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F328,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="57" priority="59">
-      <formula>(VLOOKUP(F340,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F328,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A341:I342">
+  <conditionalFormatting sqref="A329:I330">
     <cfRule type="expression" dxfId="56" priority="52">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13347,7 +12970,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A341:I342">
+  <conditionalFormatting sqref="A329:I330">
     <cfRule type="expression" dxfId="53" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13358,15 +12981,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F341:F342">
+  <conditionalFormatting sqref="F329:F330">
     <cfRule type="expression" dxfId="50" priority="50">
-      <formula>NOT(VLOOKUP(F341,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F329,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="49" priority="51">
-      <formula>(VLOOKUP(F341,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F329,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A344:I344">
+  <conditionalFormatting sqref="A332:I332">
     <cfRule type="expression" dxfId="48" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13377,7 +13000,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A344:I344">
+  <conditionalFormatting sqref="A332:I332">
     <cfRule type="expression" dxfId="45" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13388,15 +13011,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F344">
+  <conditionalFormatting sqref="F332">
     <cfRule type="expression" dxfId="42" priority="34">
-      <formula>NOT(VLOOKUP(F344,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F332,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="41" priority="35">
-      <formula>(VLOOKUP(F344,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F332,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A347:I347">
+  <conditionalFormatting sqref="A335:I335">
     <cfRule type="expression" dxfId="40" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13407,7 +13030,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A347:I347">
+  <conditionalFormatting sqref="A335:I335">
     <cfRule type="expression" dxfId="37" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13418,15 +13041,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F347">
+  <conditionalFormatting sqref="F335">
     <cfRule type="expression" dxfId="34" priority="18">
-      <formula>NOT(VLOOKUP(F347,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F335,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="19">
-      <formula>(VLOOKUP(F347,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F335,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A349:H349">
+  <conditionalFormatting sqref="A337:H337">
     <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13437,7 +13060,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A349:H349">
+  <conditionalFormatting sqref="A337:H337">
     <cfRule type="expression" dxfId="29" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13448,15 +13071,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F349">
+  <conditionalFormatting sqref="F337">
     <cfRule type="expression" dxfId="26" priority="10">
-      <formula>NOT(VLOOKUP(F349,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F337,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="11">
-      <formula>(VLOOKUP(F349,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F337,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I349">
+  <conditionalFormatting sqref="I337">
     <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -13467,7 +13090,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I349">
+  <conditionalFormatting sqref="I337">
     <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -13479,23 +13102,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F349" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F337" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E349" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E337" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G349" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G337" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H348 H20:H339" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H336 H20:H327" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H349 H340:H347" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H337 H328:H335" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"Message Deserialization, Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13505,7 +13128,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B11:B16 B18:B45 B182:B184 B186:B197 B204:B304 B320:B323 B349:B350" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B11:B16 B18:B45 B182:B184 B186:B197 B204:B303 B310:B313 B337:B338" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>